<commit_message>
- adds WebSocket Command actions - adds Probat Sample Roaster setup
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="206">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -631,6 +631,15 @@
   </si>
   <si>
     <t xml:space="preserve">for YOCTOPUCE RC modules: with r an int in %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebSocket Command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">send(&lt;json&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If {} substitutions are used, json brackets need to be duplicated to escape them like in send({{ “value”: {}}})</t>
   </si>
 </sst>
 </file>
@@ -748,7 +757,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -845,7 +854,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -944,17 +953,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A81" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C89" activeCellId="0" sqref="C89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,6 +1689,25 @@
       </c>
       <c r="C88" s="0" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds Kuban Base machine setup - adds MODBUS and S7 decoding of Floats as Integers - adds S7 Command msetDBint to write Integers to S7 registers using masks - adds S7 help page
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="208">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -469,6 +469,12 @@
   </si>
   <si>
     <t xml:space="preserve">write int to S7 DB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msetDBint(&lt;dbnumber&gt;,&lt;start&gt;,&lt;andMask&gt;,&lt;orMask&gt;,&lt;value&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write value where bits are replaced by those from orMask at positions where andMask bits are not set</t>
   </si>
   <si>
     <t xml:space="preserve">setDBfloat(&lt;dbnumber&gt;,&lt;start&gt;,&lt;value&gt;)</t>
@@ -757,7 +763,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -854,7 +860,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -953,17 +959,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A81" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C89" activeCellId="0" sqref="C89"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C61" activeCellId="0" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1458,7 +1464,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
         <v>149</v>
       </c>
@@ -1467,52 +1473,52 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="B62" s="0" t="s">
         <v>151</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="C65" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B66" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="C66" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="C66" s="0" t="s">
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
         <v>161</v>
       </c>
@@ -1530,18 +1536,18 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>52</v>
+        <v>165</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>53</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>166</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,17 +1599,17 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="B77" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="C77" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="C77" s="0" t="s">
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
         <v>182</v>
       </c>
@@ -1661,15 +1667,15 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>197</v>
+        <v>122</v>
       </c>
       <c r="C86" s="0" t="s">
         <v>198</v>
@@ -1691,22 +1697,30 @@
         <v>202</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="C89" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="C89" s="0" t="s">
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C91" s="0" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates several machine setups
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="207">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -232,9 +232,6 @@
   </si>
   <si>
     <t xml:space="preserve">write 32bit float to two 16bit int registers: MODBUS function 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">writes values to the registers in slaves specified by the given id</t>
   </si>
   <si>
     <t xml:space="preserve">DTA Command</t>
@@ -763,7 +760,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -860,7 +857,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -959,13 +956,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C61" activeCellId="0" sqref="C61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.21"/>
@@ -1122,362 +1119,362 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>70</v>
+      </c>
       <c r="B20" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="B22" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="C33" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="C34" s="0" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" s="0" t="s">
         <v>106</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="B40" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>129</v>
+      </c>
       <c r="B49" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>130</v>
-      </c>
       <c r="B50" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>135</v>
+        <v>52</v>
       </c>
       <c r="C52" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C54" s="0" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>53</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="s">
-        <v>151</v>
+      <c r="A62" s="0" t="s">
+        <v>152</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>152</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,7 +1482,7 @@
         <v>153</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,181 +1490,181 @@
         <v>154</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>157</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>160</v>
-      </c>
       <c r="B67" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>166</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>53</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>180</v>
+      </c>
       <c r="B77" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>181</v>
-      </c>
       <c r="B78" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>196</v>
+        <v>121</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>197</v>
@@ -1675,55 +1672,48 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>122</v>
+        <v>198</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>204</v>
+      </c>
       <c r="B89" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>205</v>
-      </c>
       <c r="B90" s="0" t="s">
-        <v>206</v>
+        <v>52</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C91" s="0" t="s">
         <v>53</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
- adds support for importing IKAWA v3 CSV files - adds _, {ET}, {BT}, and {time} substitution for WebSocket Commands - WebSocket Commands read and button - updates event slider and button help texts - updates Probat P Series setups - updates translations
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="212">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -192,6 +192,12 @@
     <t xml:space="preserve">sets calling button to “pressed” if argument is 1 or True</t>
   </si>
   <si>
+    <t xml:space="preserve">read(slaveID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads register from slave slaveID using function 3 (Read Multiple Holding Registers). The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
     <t xml:space="preserve">write([slaveId,register,value],..,[slaveId,register,value])</t>
   </si>
   <si>
@@ -643,6 +649,15 @@
   </si>
   <si>
     <t xml:space="preserve">If {} substitutions are used, json brackets need to be duplicated to escape them like in send({{ “value”: {}}})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets calling button to “pressed” if argument evaluates to 1 or True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read(&lt;json&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if the `&lt;json&gt;` text respects the JSON format it is send to the connected WebSocket server and the response is bound to the variable `_`</t>
   </si>
 </sst>
 </file>
@@ -757,10 +772,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B93:C94 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -854,10 +869,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="B93:C94 B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -956,17 +971,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B93" activeCellId="0" sqref="B93:C94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,7 +1077,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
         <v>56</v>
       </c>
@@ -1119,10 +1134,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="B20" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1133,11 +1148,11 @@
       <c r="B21" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="0" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>75</v>
       </c>
@@ -1227,18 +1242,18 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C34" s="0" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,19 +1264,19 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="0" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="B37" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C37" s="0" t="s">
@@ -1272,7 +1287,7 @@
       <c r="A38" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="C38" s="0" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1283,11 +1298,11 @@
       <c r="B39" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="0" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
         <v>111</v>
       </c>
@@ -1360,17 +1375,17 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="B49" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="C49" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="C49" s="0" t="s">
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
         <v>132</v>
       </c>
@@ -1388,101 +1403,101 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C53" s="0" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B53" s="0" t="s">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="C54" s="0" t="s">
-        <v>53</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>138</v>
+        <v>52</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C57" s="0" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C62" s="0" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="C62" s="0" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="C63" s="0" t="s">
         <v>153</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1490,53 +1505,53 @@
         <v>154</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>155</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>158</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B67" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="C67" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C66" s="0" t="s">
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0" t="s">
+      <c r="B68" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C68" s="0" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>52</v>
+        <v>164</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>53</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,171 +1564,202 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
-        <v>168</v>
+        <v>52</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>169</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C77" s="0" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B79" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="C79" s="0" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>121</v>
+        <v>195</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C86" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>200</v>
+        <v>123</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="C88" s="0" t="s">
+      <c r="C89" s="0" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="C90" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="C89" s="0" t="s">
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="0" t="s">
+      <c r="B91" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C92" s="0" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
adds range command action to Phidget VOUT slider and button help page
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="213">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -420,6 +420,12 @@
     <t xml:space="preserve">VOUT Command</t>
   </si>
   <si>
+    <t xml:space="preserve">range(c,r[,sn])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for PHIDGET OUTPUT modules: sets voltage voltage range (r=5 fo r5V and r=10 for 10V)</t>
+  </si>
+  <si>
     <t xml:space="preserve">out(&lt;n&gt;,&lt;v&gt;[,&lt;sn&gt;])</t>
   </si>
   <si>
@@ -634,9 +640,6 @@
   </si>
   <si>
     <t xml:space="preserve">for YOCTOPUCE RC modules: with n an int [0..65000] in us</t>
-  </si>
-  <si>
-    <t xml:space="preserve">range(c,r[,sn])</t>
   </si>
   <si>
     <t xml:space="preserve">for YOCTOPUCE RC modules: with r an int in %</t>
@@ -772,10 +775,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B93:C94 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B50:C50 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -869,10 +872,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="B93:C94 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="B50:C50 B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -971,13 +974,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C94"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B93" activeCellId="0" sqref="B93:C94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50:C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.21"/>
@@ -1382,7 +1385,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>131</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
         <v>134</v>
       </c>
@@ -1411,45 +1414,45 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C54" s="0" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="B54" s="0" t="s">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B55" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C54" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="C55" s="0" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>140</v>
+        <v>54</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>141</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1460,7 +1463,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
         <v>144</v>
       </c>
@@ -1468,7 +1471,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
         <v>146</v>
       </c>
@@ -1476,7 +1479,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
         <v>148</v>
       </c>
@@ -1484,7 +1487,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
         <v>150</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
         <v>152</v>
       </c>
@@ -1501,52 +1504,52 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="B64" s="0" t="s">
         <v>154</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>157</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="C67" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B68" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="C68" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C68" s="0" t="s">
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
         <v>164</v>
       </c>
@@ -1564,18 +1567,18 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>168</v>
+        <v>52</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>169</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1627,17 +1630,17 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="B79" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="C79" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="C79" s="0" t="s">
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
         <v>185</v>
       </c>
@@ -1695,15 +1698,15 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>123</v>
+        <v>199</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>200</v>
+        <v>123</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>201</v>
@@ -1725,39 +1728,47 @@
         <v>205</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C91" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="B91" s="0" t="s">
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="C91" s="0" t="s">
+      <c r="B92" s="0" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="C92" s="0" t="s">
-        <v>53</v>
+        <v>209</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>209</v>
+        <v>53</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C94" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="C94" s="0" t="s">
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="0" t="s">
         <v>211</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- optimized artisan.plus synchronization - adds Artisan Command to switch the button/slider palette - fixes the appRaised signal - show/hides event annotations in combo mode along the step lines on clicking the legend handles
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="233">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -616,6 +616,12 @@
   </si>
   <si>
     <t xml:space="preserve">activates button &lt;name&gt; from { START, CHARGE, DRY, FCs, FCe, SCs, SCe, DROP, COOL, OFF } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">palette(&lt;int&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activates palette &lt;int&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">playbackmode(&lt;int&gt;)</t>
@@ -829,10 +835,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B87:C87 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -926,10 +932,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="B87:C87 B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1028,13 +1034,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B79" activeCellId="0" sqref="B79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B74" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B87" activeCellId="0" sqref="B87:C87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.14"/>
@@ -1747,7 +1753,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
         <v>198</v>
       </c>
@@ -1764,17 +1770,17 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="B89" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="C89" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="C89" s="0" t="s">
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
         <v>205</v>
       </c>
@@ -1832,15 +1838,15 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="s">
-        <v>123</v>
+        <v>219</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="s">
-        <v>220</v>
+        <v>123</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>221</v>
@@ -1856,45 +1862,53 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C100" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="B101" s="0" t="s">
+      <c r="C101" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="C101" s="0" t="s">
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>52</v>
+        <v>228</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>53</v>
+        <v>229</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>228</v>
+        <v>53</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
-        <v>229</v>
+        <v>54</v>
       </c>
       <c r="C104" s="0" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds labeled alarm sets - adds Ramp/Soak pattern labels - adds option to load Ramp/Soak patterns from background profile - displays path the Ramp/Soak patterns were loaded from
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="239">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -576,10 +576,10 @@
     <t xml:space="preserve">sets the PID target set value SV</t>
   </si>
   <si>
-    <t xml:space="preserve">pidRS(&lt;int&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activates the PID Ramp-Soak pattern number &lt;n&gt; (1-based!)</t>
+    <t xml:space="preserve">pidRS(&lt;rs&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activates the PID Ramp-Soak pattern number &lt;rs&gt; (1-based!) or the one labeled &lt;rs&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">pidSource(&lt;int&gt;)</t>
@@ -618,10 +618,10 @@
     <t xml:space="preserve">activates button &lt;name&gt; from { START, CHARGE, DRY, FCs, FCe, SCs, SCe, DROP, COOL, OFF } </t>
   </si>
   <si>
-    <t xml:space="preserve">palette(&lt;int&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activates palette &lt;int&gt;</t>
+    <t xml:space="preserve">palette(&lt;p&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activates palette &lt;p&gt; with &lt;p&gt; either a number 0-9 or a palette label</t>
   </si>
   <si>
     <t xml:space="preserve">playbackmode(&lt;int&gt;)</t>
@@ -646,6 +646,12 @@
   </si>
   <si>
     <t xml:space="preserve">clears the current background profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alarmset(&lt;as&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activates the alarmset with the given number or label</t>
   </si>
   <si>
     <t xml:space="preserve">RC Command</t>
@@ -850,7 +856,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -947,7 +953,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1046,17 +1052,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C91" activeCellId="0" sqref="C91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C87" activeCellId="0" sqref="C87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,18 +1811,18 @@
         <v>207</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B92" s="0" t="s">
+      <c r="C92" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="C92" s="0" t="s">
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="s">
         <v>211</v>
       </c>
@@ -1874,15 +1880,15 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
-        <v>123</v>
+        <v>225</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>226</v>
+        <v>123</v>
       </c>
       <c r="C101" s="0" t="s">
         <v>227</v>
@@ -1898,45 +1904,53 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C103" s="0" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="B104" s="0" t="s">
+      <c r="C104" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="C104" s="0" t="s">
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
-        <v>52</v>
+        <v>234</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>53</v>
+        <v>235</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>234</v>
+        <v>53</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
-        <v>235</v>
+        <v>54</v>
       </c>
       <c r="C107" s="0" t="s">
         <v>236</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds Artisan Command adjustSV to allow for relative adjustments of the set value
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="241">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -570,7 +570,13 @@
     <t xml:space="preserve">sets the p-i-d parameters of the PID</t>
   </si>
   <si>
-    <t xml:space="preserve">pidSV(&lt;float&gt;)</t>
+    <t xml:space="preserve">adjustSV(&lt;int&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">increases or decreases the current target SV value by &lt;int&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pidSV(&lt;int&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">sets the PID target set value SV</t>
@@ -853,10 +859,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B79:C79 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -950,10 +956,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="B79:C79 B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1052,13 +1058,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C87" activeCellId="0" sqref="C87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B79" activeCellId="0" sqref="B79:C79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.14"/>
@@ -1779,7 +1785,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
         <v>200</v>
       </c>
@@ -1795,7 +1801,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
         <v>204</v>
       </c>
@@ -1819,18 +1825,18 @@
         <v>209</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="B93" s="0" t="s">
+      <c r="C93" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="C93" s="0" t="s">
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
         <v>213</v>
       </c>
@@ -1888,15 +1894,15 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>123</v>
+        <v>227</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>228</v>
+        <v>123</v>
       </c>
       <c r="C102" s="0" t="s">
         <v>229</v>
@@ -1912,45 +1918,53 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C104" s="0" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="B105" s="0" t="s">
+      <c r="C105" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="C105" s="0" t="s">
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="s">
-        <v>52</v>
+        <v>236</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>53</v>
+        <v>237</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>236</v>
+        <v>53</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>237</v>
+        <v>54</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>238</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds ArtisanCommands moveBackground and pidLookahead
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="245">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -594,6 +594,12 @@
     <t xml:space="preserve">selects the PID input source with &lt;n&gt; 0: BT, 1: ET (Software PID); &lt;n&gt; in {0,..,3} (Arduino PID)</t>
   </si>
   <si>
+    <t xml:space="preserve">pidLookahead(&lt;int&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets the PID lookahead</t>
+  </si>
+  <si>
     <t xml:space="preserve">popup(&lt;msg&gt;[,&lt;int&gt;])</t>
   </si>
   <si>
@@ -658,6 +664,12 @@
   </si>
   <si>
     <t xml:space="preserve">activates the alarmset with the given number or label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moveBackground(&lt;direction&gt;,&lt;int&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moves the background profile the indicated number of steps towards &lt;direction&gt;, with &lt;direction&gt; one of up, down, left, right</t>
   </si>
   <si>
     <t xml:space="preserve">RC Command</t>
@@ -859,10 +871,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B79:C79 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -956,10 +968,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="B79:C79 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1058,17 +1070,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B79" activeCellId="0" sqref="B79:C79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C95" activeCellId="0" sqref="C95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1793,7 +1805,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
         <v>202</v>
       </c>
@@ -1809,7 +1821,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
         <v>206</v>
       </c>
@@ -1833,26 +1845,26 @@
         <v>211</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="B94" s="0" t="s">
+      <c r="C94" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="C94" s="0" t="s">
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="0" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="0" t="s">
+      <c r="C95" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="C95" s="0" t="s">
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="s">
         <v>217</v>
       </c>
@@ -1902,23 +1914,23 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>123</v>
+        <v>229</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
-        <v>232</v>
+        <v>123</v>
       </c>
       <c r="C104" s="0" t="s">
         <v>233</v>
@@ -1926,16 +1938,13 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
-        <v>132</v>
+        <v>234</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
-        <v>235</v>
-      </c>
       <c r="B106" s="0" t="s">
         <v>236</v>
       </c>
@@ -1945,26 +1954,45 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>53</v>
+        <v>238</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>239</v>
+      </c>
       <c r="B108" s="0" t="s">
-        <v>54</v>
+        <v>240</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
-        <v>239</v>
+        <v>52</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>240</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fixes MODBUS slider action (re-activated automatic conversion of placeholder {} value to integer) - adds MODBUS Command writeSingle to force the use of MODBUS function 6 over the more general MODBUS Command write which writes integers via function 6 and floats via function 16
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="247">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -198,7 +198,7 @@
     <t xml:space="preserve">reads register from slave slaveID using function 3 (Read Multiple Holding Registers). The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
   </si>
   <si>
-    <t xml:space="preserve">write([slaveId,register,value],..,[slaveId,register,value])</t>
+    <t xml:space="preserve">write(slaveId,register,value) or write([slaveId,register,value],..,[slaveId,register,value])</t>
   </si>
   <si>
     <t xml:space="preserve">write register: MODBUS function 6 (int) or function 16 (float)</t>
@@ -231,13 +231,19 @@
     <t xml:space="preserve">writeBCD(s,r,v) or writeBCD([s,r,v],..,[s,r,v])</t>
   </si>
   <si>
-    <t xml:space="preserve">write 16bit BCD encoded value v to regiseter r of slave s </t>
-  </si>
-  <si>
-    <t xml:space="preserve">writeWord(slaveId,register,value)</t>
+    <t xml:space="preserve">write 16bit BCD encoded value v to register r of slave s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">writeWord(slaveId,register,value) or writeWord([slaveId,register,value],..,[slaveId,register,value])</t>
   </si>
   <si>
     <t xml:space="preserve">write 32bit float to two 16bit int registers: MODBUS function 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">writeSingle(slaveId,register,value) or writeSingle([slaveId,register,value],..,[slaveId,register,value])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write 16bit integer to a single 16bit register: MODBUS function 6 (int)</t>
   </si>
   <si>
     <t xml:space="preserve">DTA Command</t>
@@ -838,12 +844,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -874,7 +884,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -971,7 +981,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1070,16 +1080,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C95" activeCellId="0" sqref="C95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
   </cols>
   <sheetData>
@@ -1184,8 +1194,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+    <row r="14" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C14" s="0" t="s">
@@ -1232,7 +1242,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>70</v>
       </c>
@@ -1240,11 +1250,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1255,11 +1265,11 @@
       <c r="B22" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="0" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>77</v>
       </c>
@@ -1349,18 +1359,18 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C35" s="0" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1375,15 +1385,15 @@
       <c r="A37" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>106</v>
       </c>
       <c r="C38" s="0" t="s">
@@ -1394,7 +1404,7 @@
       <c r="A39" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="C39" s="0" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1405,11 +1415,11 @@
       <c r="B40" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C40" s="0" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
         <v>113</v>
       </c>
@@ -1482,17 +1492,17 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="B50" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="C50" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C50" s="0" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
         <v>134</v>
       </c>
@@ -1518,45 +1528,45 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C55" s="0" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="B55" s="0" t="s">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B56" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="C56" s="0" t="s">
-        <v>53</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>142</v>
+        <v>54</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>143</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,16 +1618,16 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="B65" s="0" t="s">
         <v>156</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>102</v>
@@ -1625,35 +1635,35 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>159</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="C68" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B69" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="C69" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="C69" s="0" t="s">
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
         <v>166</v>
       </c>
@@ -1671,18 +1681,18 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>53</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>170</v>
+        <v>52</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>171</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,7 +1727,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
         <v>180</v>
       </c>
@@ -1813,7 +1823,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
         <v>204</v>
       </c>
@@ -1829,7 +1839,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="s">
         <v>208</v>
       </c>
@@ -1861,18 +1871,18 @@
         <v>215</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B96" s="0" t="s">
+      <c r="C96" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="C96" s="0" t="s">
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="s">
         <v>219</v>
       </c>
@@ -1930,15 +1940,15 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
-        <v>123</v>
+        <v>233</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
-        <v>234</v>
+        <v>125</v>
       </c>
       <c r="C105" s="0" t="s">
         <v>235</v>
@@ -1954,45 +1964,53 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
-        <v>132</v>
+        <v>238</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
-        <v>239</v>
-      </c>
       <c r="B108" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C108" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="C108" s="0" t="s">
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
-        <v>52</v>
+        <v>242</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>53</v>
+        <v>243</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>242</v>
+        <v>53</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
-        <v>243</v>
+        <v>54</v>
       </c>
       <c r="C111" s="0" t="s">
         <v>244</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds {BTB} and {ETB} command substitution replacing those placeholders by the value of BT and ET of the background profile, if loaded, at the current time in Serial/CallProgram/MODBUS/S7/WebSocket command actions
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="248">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -133,6 +133,27 @@
   </si>
   <si>
     <t xml:space="preserve">tn:Note: "{}" can be used as a placeholder, it will be substituted by the current button value plus the offset for \u00B1 event types.  If a placeholder occurs several times in a description/command, all those occurrences are replaced by the value.\n</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tn:Note: The placeholders </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{ET}, {BT}, {time}, {ETB}, {BTB} will be substituted by the current ET, BT, time, ET background or BT background value in Serial/CallProgram/MODBUS/S7/WebSocket commands</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">tn:Note: commands can be sequenced, separated by semicolons like in “&lt;cmd1&gt;;&lt;cmd2&gt;;&lt;cmd3&gt;”\n</t>
@@ -772,7 +793,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -800,6 +821,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -884,7 +911,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -981,7 +1008,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1080,13 +1107,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1103,7 +1130,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>37</v>
       </c>
@@ -1120,517 +1147,514 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>42</v>
+      <c r="C7" s="0" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="B11" s="0" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="C15" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="0" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="0" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="C22" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="0" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="B24" s="0" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="C24" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="C36" s="0" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="B41" s="0" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="B42" s="0" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+      <c r="C42" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="0" t="s">
         <v>127</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="0" t="s">
         <v>129</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C50" s="0" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="C51" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="B51" s="0" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="B52" s="0" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+      <c r="C52" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="0" t="s">
         <v>140</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="C55" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="C56" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>144</v>
+        <v>55</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C61" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="C62" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C63" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C64" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C65" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="C65" s="0" t="s">
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="0" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="C66" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,7 +1662,7 @@
         <v>159</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,309 +1670,309 @@
         <v>160</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>161</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C70" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B70" s="0" t="s">
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="B71" s="0" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0" t="s">
+      <c r="C71" s="0" t="s">
         <v>168</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C72" s="0" t="s">
         <v>170</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>52</v>
+        <v>171</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>53</v>
+        <v>172</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>172</v>
+        <v>53</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>173</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" s="0" t="s">
         <v>174</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C77" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C78" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="C78" s="0" t="s">
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="0" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="0" t="s">
+      <c r="C79" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C80" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C81" s="0" t="s">
         <v>186</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C82" s="0" t="s">
         <v>188</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C83" s="0" t="s">
         <v>190</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C84" s="0" t="s">
         <v>192</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" s="0" t="s">
         <v>194</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="0" t="s">
         <v>196</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C87" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="C88" s="0" t="s">
         <v>200</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C89" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C90" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="C90" s="0" t="s">
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="0" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="0" t="s">
+      <c r="C91" s="0" t="s">
         <v>206</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C92" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="C92" s="0" t="s">
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="0" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="0" t="s">
+      <c r="C93" s="0" t="s">
         <v>210</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C94" s="0" t="s">
         <v>212</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C95" s="0" t="s">
         <v>214</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="C96" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="C96" s="0" t="s">
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="0" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="C97" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="B97" s="0" t="s">
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="C97" s="0" t="s">
+      <c r="B98" s="0" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="0" t="s">
+      <c r="C98" s="0" t="s">
         <v>221</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="C99" s="0" t="s">
         <v>223</v>
-      </c>
-      <c r="C99" s="0" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="C100" s="0" t="s">
         <v>225</v>
-      </c>
-      <c r="C100" s="0" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="C101" s="0" t="s">
         <v>227</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C102" s="0" t="s">
         <v>229</v>
-      </c>
-      <c r="C102" s="0" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C103" s="0" t="s">
         <v>231</v>
-      </c>
-      <c r="C103" s="0" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C104" s="0" t="s">
         <v>233</v>
-      </c>
-      <c r="C104" s="0" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
-        <v>125</v>
+        <v>234</v>
       </c>
       <c r="C105" s="0" t="s">
         <v>235</v>
@@ -1956,61 +1980,69 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C106" s="0" t="s">
         <v>236</v>
-      </c>
-      <c r="C106" s="0" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="C107" s="0" t="s">
         <v>238</v>
-      </c>
-      <c r="C107" s="0" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>134</v>
+        <v>239</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="B109" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C109" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="B109" s="0" t="s">
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C109" s="0" t="s">
+      <c r="B110" s="0" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="C110" s="0" t="s">
-        <v>53</v>
+        <v>244</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C111" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="C111" s="0" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C112" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="C112" s="0" t="s">
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="0" t="s">
         <v>246</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds IO Command limit(c,v[,sn]) to set the current limit on a DCMotor Phidget (Issue #626)
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="250">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -135,25 +135,7 @@
     <t xml:space="preserve">tn:Note: "{}" can be used as a placeholder, it will be substituted by the current button value plus the offset for \u00B1 event types.  If a placeholder occurs several times in a description/command, all those occurrences are replaced by the value.\n</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">tn:Note: The placeholders </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">{ET}, {BT}, {time}, {ETB}, {BTB} will be substituted by the current ET, BT, time, ET background or BT background value in Serial/CallProgram/MODBUS/S7/WebSocket commands</t>
-    </r>
+    <t xml:space="preserve">tn:Note: The placeholders {ET}, {BT}, {time}, {ETB}, {BTB} will be substituted by the current ET, BT, time, ET background, BT background value in Serial/CallProgram/MODBUS/S7/WebSocket commands\n</t>
   </si>
   <si>
     <t xml:space="preserve">tn:Note: commands can be sequenced, separated by semicolons like in “&lt;cmd1&gt;;&lt;cmd2&gt;;&lt;cmd3&gt;”\n</t>
@@ -310,6 +292,12 @@
   </si>
   <si>
     <t xml:space="preserve">PHIDGET DCMotor: sets target velocity of channel c to v (float)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limit(c,v[,sn])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHIDGET DCMotor: sets current limit of channel c to v (float)</t>
   </si>
   <si>
     <t xml:space="preserve">on(c[,sn])</t>
@@ -793,7 +781,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -821,12 +809,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -911,7 +893,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1008,7 +990,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1107,13 +1089,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1130,7 +1112,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>37</v>
       </c>
@@ -1349,8 +1331,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C30" s="0" t="s">
@@ -1399,18 +1381,18 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C37" s="0" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1425,15 +1407,15 @@
       <c r="A39" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C40" s="0" t="s">
@@ -1444,7 +1426,7 @@
       <c r="A41" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="C41" s="0" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1455,11 +1437,11 @@
       <c r="B42" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="C42" s="0" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>116</v>
       </c>
@@ -1532,17 +1514,17 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="B52" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="C52" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C52" s="0" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
         <v>137</v>
       </c>
@@ -1568,45 +1550,45 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C57" s="0" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="B57" s="0" t="s">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="0" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="C58" s="0" t="s">
-        <v>54</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,16 +1640,16 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="B67" s="0" t="s">
         <v>159</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>105</v>
@@ -1675,35 +1657,35 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>162</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="C70" s="0" t="s">
         <v>164</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B71" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="C71" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="C71" s="0" t="s">
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
         <v>169</v>
       </c>
@@ -1721,18 +1703,18 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>53</v>
+        <v>173</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>54</v>
+        <v>174</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>173</v>
+        <v>53</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>174</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,7 +1749,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
         <v>183</v>
       </c>
@@ -1863,7 +1845,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="0" t="s">
         <v>207</v>
       </c>
@@ -1879,7 +1861,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
         <v>211</v>
       </c>
@@ -1911,18 +1893,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B98" s="0" t="s">
+      <c r="C98" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="C98" s="0" t="s">
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="s">
         <v>222</v>
       </c>
@@ -1980,15 +1962,15 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="s">
-        <v>126</v>
+        <v>236</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
-        <v>237</v>
+        <v>128</v>
       </c>
       <c r="C107" s="0" t="s">
         <v>238</v>
@@ -2004,45 +1986,53 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
-        <v>135</v>
+        <v>241</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
-        <v>242</v>
-      </c>
       <c r="B110" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C110" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="C110" s="0" t="s">
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
-        <v>53</v>
+        <v>245</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>54</v>
+        <v>246</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>245</v>
+        <v>54</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>246</v>
+        <v>55</v>
       </c>
       <c r="C113" s="0" t="s">
         <v>247</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds Artisan Command "keyboard" to enable/disable keyboard mode - keep ambient phidgets attached until app termination - removes Probat Middleware support - recovers lost zh_TW translations - small optimizations
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="252">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -685,6 +685,12 @@
   </si>
   <si>
     <t xml:space="preserve">moves the background profile the indicated number of steps towards &lt;direction&gt;, with &lt;direction&gt; one of up, down, left, right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keyboard(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enables/disables keyboard mode</t>
   </si>
   <si>
     <t xml:space="preserve">RC Command</t>
@@ -883,7 +889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -893,7 +899,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -971,7 +977,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -980,7 +986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -990,7 +996,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1076,7 +1082,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1085,21 +1091,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C99" activeCellId="0" sqref="C99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,18 +1907,18 @@
         <v>220</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="C99" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="C99" s="0" t="s">
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
         <v>224</v>
       </c>
@@ -1970,15 +1976,15 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
-        <v>128</v>
+        <v>238</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>239</v>
+        <v>128</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>240</v>
@@ -1994,51 +2000,60 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C110" s="0" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="B111" s="0" t="s">
+      <c r="C111" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="C111" s="0" t="s">
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="s">
-        <v>53</v>
+        <v>247</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>54</v>
+        <v>248</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>247</v>
+        <v>54</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>248</v>
+        <v>55</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>249</v>
       </c>
     </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
adds Artisan Commands `showCurve`, `showExtraCurve`, `showEvents`, and `showBackgroundEvents` to show/hide curves and events
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="260">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -691,6 +691,30 @@
   </si>
   <si>
     <t xml:space="preserve">enables/disables keyboard mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showCurve(&lt;name&gt;,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the curve indicated by &lt;name&gt; which is one of { ET, BT, DeltaET, DeltaBT, BackgroundET, BackgroundBT}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showExtraCurve(&lt;extra_device&gt;,&lt;curve&gt;,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the &lt;curve&gt; (one of {T1,T2}) of the zero-based &lt;extra_device&gt; number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showEvents(&lt;event_type&gt;, &lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the events of &lt;event_type&gt; in [1,..,5]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showBackgroundEvents(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the events of the background profile</t>
   </si>
   <si>
     <t xml:space="preserve">RC Command</t>
@@ -899,7 +923,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -996,7 +1020,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1095,13 +1119,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C99" activeCellId="0" sqref="C99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C101" activeCellId="0" sqref="C101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1915,42 +1939,42 @@
         <v>222</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="B100" s="0" t="s">
+      <c r="C100" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="C100" s="0" t="s">
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="0" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="0" t="s">
+      <c r="C101" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="C101" s="0" t="s">
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="0" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="0" t="s">
+      <c r="C102" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="C102" s="0" t="s">
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="0" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="0" t="s">
+      <c r="C103" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="C103" s="0" t="s">
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
         <v>232</v>
       </c>
@@ -1984,42 +2008,39 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>128</v>
+        <v>240</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
-        <v>137</v>
+        <v>246</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
-        <v>246</v>
-      </c>
       <c r="B112" s="0" t="s">
-        <v>247</v>
+        <v>128</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>248</v>
@@ -2027,29 +2048,63 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>53</v>
+        <v>249</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>54</v>
+        <v>250</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>55</v>
+        <v>251</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>250</v>
+        <v>137</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
- adds fixes for MPL 3.5 - adds documentation of notify() Artisan Command - makes the dog happy
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="262">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -625,6 +625,12 @@
   </si>
   <si>
     <t xml:space="preserve">shows message &lt;msg&gt; in the message line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notify(&lt;title&gt;,[&lt;msg&gt;])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sends notification with title &lt;title&gt; and optional message &lt;msg&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">setCanvasColor(&lt;color&gt;)</t>
@@ -920,10 +926,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B89:C89 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1017,10 +1023,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="B89:C89 B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1119,13 +1125,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C101" activeCellId="0" sqref="C101"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B89" activeCellId="0" sqref="B89:C89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1883,7 +1889,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="0" t="s">
         <v>209</v>
       </c>
@@ -1899,7 +1905,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="s">
         <v>213</v>
       </c>
@@ -1971,18 +1977,18 @@
         <v>230</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="B104" s="0" t="s">
+      <c r="C104" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="C104" s="0" t="s">
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
         <v>234</v>
       </c>
@@ -2040,15 +2046,15 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="s">
-        <v>128</v>
+        <v>248</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>249</v>
+        <v>128</v>
       </c>
       <c r="C113" s="0" t="s">
         <v>250</v>
@@ -2064,45 +2070,53 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C115" s="0" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="B116" s="0" t="s">
+      <c r="C116" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="C116" s="0" t="s">
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="0" t="s">
-        <v>53</v>
+        <v>257</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>54</v>
+        <v>258</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>257</v>
+        <v>54</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>258</v>
+        <v>55</v>
       </c>
       <c r="C119" s="0" t="s">
         <v>259</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds notifications - minor fixes and speed improvements
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="264">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -625,6 +625,12 @@
   </si>
   <si>
     <t xml:space="preserve">shows message &lt;msg&gt; in the message line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notifications(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enables/disables notifications; while disabled issued notifications are ignored</t>
   </si>
   <si>
     <t xml:space="preserve">notify(&lt;title&gt;,[&lt;msg&gt;])</t>
@@ -929,7 +935,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B89:C89 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1026,7 +1032,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="B89:C89 B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1125,13 +1131,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B89" activeCellId="0" sqref="B89:C89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1897,7 +1903,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="0" t="s">
         <v>211</v>
       </c>
@@ -1913,7 +1919,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="s">
         <v>215</v>
       </c>
@@ -1985,18 +1991,18 @@
         <v>232</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="B105" s="0" t="s">
+      <c r="C105" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="C105" s="0" t="s">
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="0" t="s">
         <v>236</v>
       </c>
@@ -2054,15 +2060,15 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>251</v>
+        <v>128</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>252</v>
@@ -2078,45 +2084,53 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C116" s="0" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="B117" s="0" t="s">
+      <c r="C117" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="C117" s="0" t="s">
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="0" t="s">
-        <v>53</v>
+        <v>259</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>54</v>
+        <v>260</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>259</v>
+        <v>54</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="s">
-        <v>260</v>
+        <v>55</v>
       </c>
       <c r="C120" s="0" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds Modbus Command "writeLong" to send a 32bit integer to the connected MODBUS device
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="266">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t xml:space="preserve">write 32bit float to two 16bit int registers: MODBUS function 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">writeLong(slaveId,register,value) or writeLong([slaveId,register,value],..,[slaveId,register,value])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write 32bit integer to two 16bit int registers: MODBUS function 16</t>
   </si>
   <si>
     <t xml:space="preserve">writeSingle(slaveId,register,value) or writeSingle([slaveId,register,value],..,[slaveId,register,value])</t>
@@ -932,10 +938,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B89:C89 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1029,10 +1035,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="B89:C89 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1131,13 +1137,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B89" activeCellId="0" sqref="B89:C89"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1298,7 +1304,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>71</v>
       </c>
@@ -1306,7 +1312,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>73</v>
       </c>
@@ -1314,11 +1320,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="C23" s="0" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1329,11 +1335,11 @@
       <c r="B24" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="0" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
         <v>80</v>
       </c>
@@ -1373,16 +1379,16 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="2" t="s">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
         <v>90</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C31" s="0" t="s">
@@ -1431,18 +1437,18 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C38" s="0" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1457,15 +1463,15 @@
       <c r="A40" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="C40" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>111</v>
       </c>
       <c r="C41" s="0" t="s">
@@ -1476,7 +1482,7 @@
       <c r="A42" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="C42" s="0" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1487,11 +1493,11 @@
       <c r="B43" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="C43" s="0" t="s">
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>118</v>
       </c>
@@ -1564,17 +1570,17 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="B53" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="C53" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C53" s="0" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
         <v>139</v>
       </c>
@@ -1600,45 +1606,45 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C58" s="0" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B58" s="0" t="s">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="C59" s="0" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>147</v>
+        <v>55</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>148</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,16 +1696,16 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="B68" s="0" t="s">
         <v>161</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>105</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>107</v>
@@ -1707,35 +1713,35 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>164</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="C71" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="C72" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="C72" s="0" t="s">
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
         <v>171</v>
       </c>
@@ -1753,18 +1759,18 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>175</v>
+        <v>53</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>176</v>
+        <v>54</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,7 +1805,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
         <v>185</v>
       </c>
@@ -1911,7 +1917,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="0" t="s">
         <v>213</v>
       </c>
@@ -1927,7 +1933,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="s">
         <v>217</v>
       </c>
@@ -1999,18 +2005,18 @@
         <v>234</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="B106" s="0" t="s">
+      <c r="C106" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="C106" s="0" t="s">
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
         <v>238</v>
       </c>
@@ -2068,15 +2074,15 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>128</v>
+        <v>252</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>253</v>
+        <v>130</v>
       </c>
       <c r="C115" s="0" t="s">
         <v>254</v>
@@ -2092,45 +2098,53 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="0" t="s">
-        <v>137</v>
+        <v>257</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
-        <v>258</v>
-      </c>
       <c r="B118" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C118" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="C118" s="0" t="s">
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>53</v>
+        <v>261</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>54</v>
+        <v>262</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>261</v>
+        <v>54</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="0" t="s">
-        <v>262</v>
+        <v>55</v>
       </c>
       <c r="C121" s="0" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds Artisan Command keepON(<bool>) - upgrades to pymodbus 3.0 - fixes event step line extension to CHARGE in case event snap, 100%-step and showFull were disabled and implemented the mechanism also for the background profile
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="268">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -709,6 +709,12 @@
   </si>
   <si>
     <t xml:space="preserve">enables/disables keyboard mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keepON(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enables/disables the Keep ON flag</t>
   </si>
   <si>
     <t xml:space="preserve">showCurve(&lt;name&gt;,&lt;bool&gt;)</t>
@@ -941,7 +947,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1038,7 +1044,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1137,17 +1143,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C122"/>
+  <dimension ref="A1:C123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A86" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C103" activeCellId="0" sqref="C103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2013,18 +2019,18 @@
         <v>236</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="B107" s="0" t="s">
+      <c r="C107" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="C107" s="0" t="s">
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
         <v>240</v>
       </c>
@@ -2082,15 +2088,15 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>130</v>
+        <v>254</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
-        <v>255</v>
+        <v>130</v>
       </c>
       <c r="C116" s="0" t="s">
         <v>256</v>
@@ -2106,45 +2112,53 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="C118" s="0" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="B119" s="0" t="s">
+      <c r="C119" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="C119" s="0" t="s">
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="0" t="s">
-        <v>53</v>
+        <v>263</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>54</v>
+        <v>264</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>263</v>
+        <v>54</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="0" t="s">
-        <v>264</v>
+        <v>55</v>
       </c>
       <c r="C122" s="0" t="s">
         <v>265</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fixes S7 and MODBUS read commands which may fail due to cache misses breaking control on some machines like Probatone and Kirsch & Mauser (Issue #1002) - adds MODBUS Commands readBCD, read32, read32Signed, read32BCD, and readFloat - updates keep-alive ping frequency on Probat setups
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="280">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -198,7 +198,43 @@
     <t xml:space="preserve">read(slaveID,register)</t>
   </si>
   <si>
-    <t xml:space="preserve">reads register from slave slaveID using function 3 (Read Multiple Holding Registers). The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+    <t xml:space="preserve">reads 1 16bit register from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as unsigned integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">readSigned(slaveId,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 1 16bit register from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as signed integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">readBCD(slaveID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 1 16bit register from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as BCD. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read32(slaveID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit registers from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as unsigned integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read32Signed(slaveID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit registers from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as signed integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read32BCD(slaveID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit register from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as BCD. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">readFloat(slaveID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit registers from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as float. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
   </si>
   <si>
     <t xml:space="preserve">write(slaveId,register,value) or write([slaveId,register,value],..,[slaveId,register,value])</t>
@@ -947,7 +983,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1044,7 +1080,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1143,17 +1179,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A86" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C103" activeCellId="0" sqref="C103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,15 +1298,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
         <v>61</v>
       </c>
@@ -1278,7 +1314,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
         <v>63</v>
       </c>
@@ -1286,7 +1322,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>65</v>
       </c>
@@ -1294,7 +1330,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
         <v>67</v>
       </c>
@@ -1302,7 +1338,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>69</v>
       </c>
@@ -1310,15 +1346,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+    <row r="21" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>73</v>
       </c>
@@ -1326,7 +1362,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>75</v>
       </c>
@@ -1335,66 +1371,66 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="B24" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="C24" s="0" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="B25" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="C25" s="0" t="s">
         <v>80</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="0" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="C27" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="0" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="C28" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="0" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="C29" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="0" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="0" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="0" t="s">
         <v>92</v>
       </c>
       <c r="C31" s="0" t="s">
@@ -1441,8 +1477,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C37" s="0" t="s">
@@ -1451,107 +1487,107 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>106</v>
+      <c r="B39" s="0" t="s">
+        <v>108</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>108</v>
+      <c r="B40" s="0" t="s">
+        <v>110</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>111</v>
+      <c r="B41" s="0" t="s">
+        <v>112</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>113</v>
+      <c r="B42" s="0" t="s">
+        <v>114</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>115</v>
-      </c>
       <c r="B43" s="0" t="s">
         <v>116</v>
       </c>
+      <c r="C43" s="0" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>117</v>
-      </c>
       <c r="B44" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C45" s="0" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C46" s="0" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="B47" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+      <c r="C47" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="C47" s="0" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0" t="s">
+      <c r="C48" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C48" s="0" t="s">
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="C49" s="0" t="s">
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
         <v>130</v>
       </c>
@@ -1584,121 +1620,121 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="B54" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="C54" s="0" t="s">
         <v>139</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C56" s="0" t="s">
         <v>143</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" s="0" t="s">
         <v>145</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>54</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>147</v>
-      </c>
       <c r="B59" s="0" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>150</v>
+      </c>
       <c r="B60" s="0" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>54</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>56</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>153</v>
+        <v>53</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>154</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>159</v>
+      </c>
       <c r="B65" s="0" t="s">
-        <v>155</v>
+        <v>51</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
-        <v>157</v>
+        <v>53</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>159</v>
+        <v>55</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>160</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,44 +1746,38 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="B69" s="0" t="s">
         <v>163</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>164</v>
+      <c r="B70" s="0" t="s">
+        <v>165</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>109</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>165</v>
+      <c r="B71" s="0" t="s">
+        <v>167</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
-        <v>167</v>
-      </c>
       <c r="B72" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>170</v>
-      </c>
       <c r="B73" s="0" t="s">
         <v>171</v>
       </c>
@@ -1764,23 +1794,23 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="0" t="s">
+      <c r="A75" s="0" t="s">
         <v>175</v>
       </c>
       <c r="C75" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="C76" s="0" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0" t="s">
+      <c r="A77" s="0" t="s">
         <v>177</v>
       </c>
       <c r="C77" s="0" t="s">
@@ -1788,46 +1818,52 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>179</v>
+      </c>
       <c r="B78" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>182</v>
+      </c>
       <c r="B79" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="s">
-        <v>187</v>
+        <v>53</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
         <v>189</v>
       </c>
@@ -1835,7 +1871,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
         <v>191</v>
       </c>
@@ -1843,7 +1879,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
         <v>193</v>
       </c>
@@ -1851,7 +1887,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
         <v>195</v>
       </c>
@@ -1859,7 +1895,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
         <v>197</v>
       </c>
@@ -1931,7 +1967,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="0" t="s">
         <v>215</v>
       </c>
@@ -1939,7 +1975,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="0" t="s">
         <v>217</v>
       </c>
@@ -1979,7 +2015,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
         <v>227</v>
       </c>
@@ -1987,7 +2023,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
         <v>229</v>
       </c>
@@ -2027,58 +2063,58 @@
         <v>238</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="B108" s="0" t="s">
+      <c r="C108" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="C108" s="0" t="s">
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="0" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="0" t="s">
+      <c r="C109" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C109" s="0" t="s">
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="0" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="0" t="s">
+      <c r="C110" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="C110" s="0" t="s">
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="0" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="0" t="s">
+      <c r="C111" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="C111" s="0" t="s">
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="0" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="0" t="s">
+      <c r="C112" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="C112" s="0" t="s">
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="0" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="0" t="s">
+      <c r="C113" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="C113" s="0" t="s">
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
         <v>252</v>
       </c>
@@ -2096,71 +2132,120 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
-        <v>130</v>
+        <v>256</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>139</v>
+        <v>262</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
-        <v>262</v>
-      </c>
       <c r="B120" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="0" t="s">
-        <v>53</v>
+        <v>266</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>54</v>
+        <v>267</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="0" t="s">
-        <v>55</v>
+        <v>142</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>267</v>
-      </c>
-    </row>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B127" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B128" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B129" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
- adds Yocto Power, Yocto Energy, Yocto Voltage and Yocto Current device types supporting the Yocto-Watt module - adds the generic Yocto Sensor device type - adds IO Command: powerReset([sn]) to reset the power counter of the Yocto-Watt module - updates the output program using aw.call_prog_with_args
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="282">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t xml:space="preserve">YOCTOPUCE Relay Output: pulse the channel c on after a delay of delay milliseconds for the duration of duration milliseconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powerReset([sn])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOCTOPUCE resets the power counter of the Yocto-Watt module</t>
   </si>
   <si>
     <t xml:space="preserve">slider(c,v)</t>
@@ -983,7 +989,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1080,7 +1086,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1179,13 +1185,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1517,7 +1523,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>114</v>
       </c>
@@ -1535,18 +1541,18 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C45" s="0" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1561,15 +1567,15 @@
       <c r="A47" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C48" s="0" t="s">
@@ -1580,7 +1586,7 @@
       <c r="A49" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="C49" s="0" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1591,11 +1597,11 @@
       <c r="B50" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="0" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
         <v>132</v>
       </c>
@@ -1668,17 +1674,17 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="B60" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="C60" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="C60" s="0" t="s">
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
         <v>153</v>
       </c>
@@ -1704,45 +1710,45 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C65" s="0" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="B65" s="0" t="s">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B66" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C65" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="C66" s="0" t="s">
-        <v>54</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>161</v>
+        <v>55</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>162</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1794,16 +1800,16 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="B75" s="0" t="s">
         <v>175</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>121</v>
@@ -1811,35 +1817,35 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>178</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="C78" s="0" t="s">
         <v>180</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B79" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="C79" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="C79" s="0" t="s">
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
         <v>185</v>
       </c>
@@ -1857,18 +1863,18 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="s">
-        <v>53</v>
+        <v>189</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>54</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>189</v>
+        <v>53</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>190</v>
+        <v>54</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,7 +1909,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
         <v>199</v>
       </c>
@@ -2015,7 +2021,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
         <v>227</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
         <v>231</v>
       </c>
@@ -2111,18 +2117,18 @@
         <v>250</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="B114" s="0" t="s">
+      <c r="C114" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="C114" s="0" t="s">
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
         <v>254</v>
       </c>
@@ -2180,15 +2186,15 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="0" t="s">
-        <v>142</v>
+        <v>268</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="0" t="s">
-        <v>269</v>
+        <v>144</v>
       </c>
       <c r="C123" s="0" t="s">
         <v>270</v>
@@ -2204,48 +2210,55 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="0" t="s">
-        <v>151</v>
+        <v>273</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
-        <v>274</v>
-      </c>
       <c r="B126" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C126" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="C126" s="0" t="s">
+    </row>
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="0" t="s">
-        <v>53</v>
+        <v>277</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>54</v>
+        <v>278</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>277</v>
+        <v>54</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="0" t="s">
-        <v>278</v>
+        <v>55</v>
       </c>
       <c r="C129" s="0" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B130" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
- disconnect MODBUS serial on IO Errors only - adds Phidget DAQ1500 support - adds Santoker Q Series and R Series support - removes Python 3.7 support and thus support for RPi Buster
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="284">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -382,6 +382,12 @@
   </si>
   <si>
     <t xml:space="preserve">switches channel c off (b=0) and on (b=1) and sets button i to pressed or normal depending on the value b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">santoker(&lt;target&gt;,&lt;value&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sends integer &lt;value&gt; to &lt;target&gt; register specified by as byte in hex notation like “fa” via the Santoker Network protocol</t>
   </si>
   <si>
     <t xml:space="preserve">Hottop Heater</t>
@@ -989,7 +995,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1086,7 +1092,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1185,17 +1191,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C130"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
+      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,8 +1561,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
         <v>120</v>
       </c>
       <c r="C46" s="0" t="s">
@@ -1575,15 +1581,15 @@
       <c r="A48" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="C48" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>127</v>
       </c>
       <c r="C49" s="0" t="s">
@@ -1594,7 +1600,7 @@
       <c r="A50" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="C50" s="0" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1605,11 +1611,11 @@
       <c r="B51" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C51" s="0" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
         <v>134</v>
       </c>
@@ -1682,17 +1688,17 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="B61" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="C61" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C61" s="0" t="s">
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
         <v>155</v>
       </c>
@@ -1718,45 +1724,45 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C66" s="0" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B66" s="0" t="s">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B67" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C66" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="C67" s="0" t="s">
-        <v>54</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>163</v>
+        <v>55</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>164</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,16 +1814,16 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="B76" s="0" t="s">
         <v>177</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>123</v>
@@ -1825,35 +1831,35 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>180</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="C79" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B80" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="C80" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="C80" s="0" t="s">
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
         <v>187</v>
       </c>
@@ -1871,18 +1877,18 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>53</v>
+        <v>191</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>54</v>
+        <v>192</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>191</v>
+        <v>53</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>192</v>
+        <v>54</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,7 +1923,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
         <v>201</v>
       </c>
@@ -2029,7 +2035,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
         <v>229</v>
       </c>
@@ -2045,7 +2051,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="0" t="s">
         <v>233</v>
       </c>
@@ -2125,18 +2131,18 @@
         <v>252</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="B115" s="0" t="s">
+      <c r="C115" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="C115" s="0" t="s">
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
         <v>256</v>
       </c>
@@ -2194,15 +2200,15 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="0" t="s">
-        <v>144</v>
+        <v>270</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="0" t="s">
-        <v>271</v>
+        <v>146</v>
       </c>
       <c r="C124" s="0" t="s">
         <v>272</v>
@@ -2218,45 +2224,53 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="0" t="s">
-        <v>153</v>
+        <v>275</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
-        <v>276</v>
-      </c>
       <c r="B127" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C127" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="C127" s="0" t="s">
+    </row>
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="0" t="s">
-        <v>53</v>
+        <v>279</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>54</v>
+        <v>280</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>279</v>
+        <v>54</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="0" t="s">
-        <v>280</v>
+        <v>55</v>
       </c>
       <c r="C130" s="0" t="s">
         <v>281</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B131" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- update minimum required OS version to macOS 11 - re-enabled MODBUS device logging - updates translations
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -1006,7 +1006,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1103,7 +1103,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1204,11 +1204,11 @@
   </sheetPr>
   <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P24" activeCellId="0" sqref="P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1286,11 +1286,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C11" s="0" t="s">

</xml_diff>

<commit_message>
- updated machine setups (Besca automatic and full automatic, Giesen, Hottop KN-8828B-2K+, Kuban Supreme Automatic, NOR A Series, Probat P Series III, Twino Ozstar) to take advantage of button label translations - renames button state substitution variable from ^ to $
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="333">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -295,7 +295,7 @@
     <t xml:space="preserve">variable holding the last value read via MODBUS</t>
   </si>
   <si>
-    <t xml:space="preserve">^</t>
+    <t xml:space="preserve">$</t>
   </si>
   <si>
     <t xml:space="preserve">variable holding the last state of the button pressed (1 or 0)</t>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t xml:space="preserve">IO Command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable holding the last result value</t>
   </si>
   <si>
     <t xml:space="preserve">set(c,b[,sn])</t>
@@ -1148,11 +1151,11 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1255,7 +1258,7 @@
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
@@ -1376,7 +1379,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1524,17 +1527,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C148"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A128" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B143" activeCellId="0" sqref="B143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="105.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="102.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1800,457 +1803,457 @@
         <v>134</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="3" t="s">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>136</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="0" t="s">
         <v>139</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="0" t="s">
         <v>143</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40" s="0" t="s">
         <v>145</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="0" t="s">
         <v>147</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>153</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C47" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C48" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C50" s="0" t="s">
+    <row r="51" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="3" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="C51" s="0" t="s">
-        <v>99</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="3" t="s">
-        <v>165</v>
+        <v>92</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>166</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C54" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="C54" s="0" t="s">
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="C55" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C56" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="C56" s="0" t="s">
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="C57" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B57" s="4" t="s">
+    </row>
+    <row r="58" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="B58" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="C58" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C59" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B60" s="3" t="s">
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="B61" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="3" t="s">
+      <c r="C61" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" s="0" t="s">
         <v>186</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="0" t="s">
         <v>188</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C64" s="0" t="s">
         <v>190</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C65" s="0" t="s">
         <v>192</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C66" s="0" t="s">
         <v>194</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C67" s="0" t="s">
         <v>196</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C69" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="C69" s="0" t="s">
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="3" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="C70" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="B70" s="3" t="s">
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="B71" s="3" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="3" t="s">
+      <c r="C71" s="0" t="s">
         <v>205</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C72" s="0" t="s">
         <v>207</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C73" s="0" t="s">
         <v>209</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="C75" s="0" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="B75" s="3" t="s">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C75" s="0" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="C76" s="0" t="s">
-        <v>91</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="3" t="s">
-        <v>213</v>
+        <v>98</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>214</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C82" s="0" t="s">
         <v>215</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C83" s="0" t="s">
         <v>217</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C84" s="0" t="s">
         <v>219</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C85" s="0" t="s">
         <v>221</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C86" s="0" t="s">
         <v>223</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C87" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="C87" s="0" t="s">
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="C88" s="0" t="s">
         <v>227</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2258,7 +2261,7 @@
         <v>228</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2266,397 +2269,397 @@
         <v>229</v>
       </c>
       <c r="C90" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="C91" s="0" t="s">
         <v>231</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C92" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="B92" s="3" t="s">
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="0" t="s">
+      <c r="C93" s="0" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C94" s="0" t="s">
         <v>237</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C95" s="0" t="s">
         <v>239</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="3" t="s">
-        <v>92</v>
+        <v>240</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>93</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="3" t="s">
-        <v>241</v>
+        <v>92</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>242</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C98" s="0" t="s">
         <v>243</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C99" s="0" t="s">
         <v>245</v>
-      </c>
-      <c r="C99" s="0" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C100" s="0" t="s">
         <v>247</v>
-      </c>
-      <c r="C100" s="0" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C101" s="0" t="s">
         <v>249</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C102" s="0" t="s">
         <v>251</v>
-      </c>
-      <c r="C102" s="0" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C103" s="0" t="s">
         <v>253</v>
-      </c>
-      <c r="C103" s="0" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C104" s="0" t="s">
         <v>255</v>
-      </c>
-      <c r="C104" s="0" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C105" s="0" t="s">
         <v>257</v>
-      </c>
-      <c r="C105" s="0" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C106" s="0" t="s">
         <v>259</v>
-      </c>
-      <c r="C106" s="0" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C107" s="0" t="s">
         <v>261</v>
-      </c>
-      <c r="C107" s="0" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C108" s="0" t="s">
         <v>263</v>
-      </c>
-      <c r="C108" s="0" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C109" s="0" t="s">
         <v>265</v>
-      </c>
-      <c r="C109" s="0" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C110" s="0" t="s">
         <v>267</v>
-      </c>
-      <c r="C110" s="0" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C111" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="C111" s="0" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C112" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="C112" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C113" s="0" t="s">
         <v>273</v>
-      </c>
-      <c r="C113" s="0" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="C115" s="0" t="s">
+    <row r="116" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="3" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="C116" s="0" t="s">
-        <v>99</v>
+        <v>277</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="3" t="s">
-        <v>277</v>
+        <v>98</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>278</v>
+        <v>99</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C118" s="0" t="s">
         <v>279</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C119" s="0" t="s">
         <v>281</v>
-      </c>
-      <c r="C119" s="0" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C120" s="0" t="s">
         <v>283</v>
-      </c>
-      <c r="C120" s="0" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C121" s="0" t="s">
         <v>285</v>
-      </c>
-      <c r="C121" s="0" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C122" s="0" t="s">
         <v>287</v>
-      </c>
-      <c r="C122" s="0" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C123" s="0" t="s">
         <v>289</v>
-      </c>
-      <c r="C123" s="0" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C124" s="0" t="s">
         <v>291</v>
-      </c>
-      <c r="C124" s="0" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C125" s="0" t="s">
         <v>293</v>
-      </c>
-      <c r="C125" s="0" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C126" s="0" t="s">
         <v>295</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C127" s="0" t="s">
         <v>297</v>
-      </c>
-      <c r="C127" s="0" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C128" s="0" t="s">
         <v>299</v>
-      </c>
-      <c r="C128" s="0" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C129" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="C129" s="0" t="s">
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B130" s="3" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
+      <c r="C130" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="B130" s="3" t="s">
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="C130" s="0" t="s">
+      <c r="B131" s="3" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B131" s="3" t="s">
+      <c r="C131" s="0" t="s">
         <v>306</v>
-      </c>
-      <c r="C131" s="0" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C132" s="0" t="s">
         <v>308</v>
-      </c>
-      <c r="C132" s="0" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C133" s="0" t="s">
         <v>310</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C134" s="0" t="s">
         <v>312</v>
-      </c>
-      <c r="C134" s="0" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C135" s="0" t="s">
         <v>314</v>
-      </c>
-      <c r="C135" s="0" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C136" s="0" t="s">
         <v>316</v>
-      </c>
-      <c r="C136" s="0" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C137" s="0" t="s">
         <v>318</v>
-      </c>
-      <c r="C137" s="0" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="3" t="s">
-        <v>194</v>
+        <v>319</v>
       </c>
       <c r="C138" s="0" t="s">
         <v>320</v>
@@ -2664,85 +2667,93 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C139" s="0" t="s">
         <v>321</v>
-      </c>
-      <c r="C139" s="0" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C140" s="0" t="s">
         <v>323</v>
-      </c>
-      <c r="C140" s="0" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="3" t="s">
-        <v>203</v>
+        <v>324</v>
       </c>
       <c r="C141" s="0" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="s">
+      <c r="B142" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C142" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="B142" s="3" t="s">
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C142" s="0" t="s">
+      <c r="C143" s="0" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B143" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="C143" s="0" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="3" t="s">
-        <v>92</v>
+        <v>328</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>93</v>
+        <v>329</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C146" s="0" t="s">
-        <v>329</v>
+        <v>94</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>99</v>
+        <v>330</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>330</v>
+        <v>98</v>
       </c>
       <c r="C148" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B149" s="3" t="s">
         <v>331</v>
+      </c>
+      <c r="C149" s="0" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- correctly removes background profile from ranking reports - fixes typo in energy entry of ranking reports - adds YOCTOPUCE relay IO Command "yset"
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="335">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -485,6 +485,12 @@
   </si>
   <si>
     <t xml:space="preserve">YOCTOPUCE Relay Output: turn channel c of the relay module off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yset(c,b[,sn])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOCTOPUCE Relay Output: switches channel c of the relay module off (b=0) and on (b=1)</t>
   </si>
   <si>
     <t xml:space="preserve">flip(c[,sn])</t>
@@ -1152,10 +1158,10 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B45:C45 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1255,10 +1261,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="1" sqref="B45:C45 B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
@@ -1376,10 +1382,10 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B45:C45 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1527,13 +1533,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A128" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B143" activeCellId="0" sqref="B143"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45:C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1931,42 +1937,42 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="3" t="s">
-        <v>98</v>
+        <v>166</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>99</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="3" t="s">
-        <v>166</v>
+        <v>92</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1977,8 +1983,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="3" t="s">
         <v>170</v>
       </c>
       <c r="C56" s="0" t="s">
@@ -1993,33 +1999,33 @@
         <v>173</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="C58" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="C58" s="0" t="s">
+    </row>
+    <row r="59" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="B59" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="0" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2030,11 +2036,11 @@
       <c r="B61" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C61" s="0" t="s">
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="3" t="s">
         <v>185</v>
       </c>
@@ -2107,17 +2113,17 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="B71" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="C71" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="C71" s="0" t="s">
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="3" t="s">
         <v>206</v>
       </c>
@@ -2143,69 +2149,69 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C76" s="0" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B76" s="3" t="s">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="0" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="C77" s="0" t="s">
-        <v>91</v>
+        <v>215</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="3" t="s">
-        <v>214</v>
+        <v>98</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>215</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,17 +2262,17 @@
         <v>227</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="3" t="s">
         <v>228</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>171</v>
+        <v>229</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>173</v>
@@ -2274,40 +2280,40 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="C92" s="0" t="s">
         <v>233</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="C93" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="0" t="s">
+      <c r="C94" s="0" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2328,18 +2334,18 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="3" t="s">
-        <v>92</v>
+        <v>242</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>93</v>
+        <v>243</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="3" t="s">
-        <v>242</v>
+        <v>92</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>243</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2472,34 +2478,34 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C116" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="C116" s="0" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="3" t="s">
-        <v>98</v>
+        <v>278</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>99</v>
+        <v>279</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="3" t="s">
-        <v>278</v>
+        <v>98</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>279</v>
+        <v>99</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2599,17 +2605,17 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
+      <c r="B131" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="B131" s="3" t="s">
+      <c r="C131" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="C131" s="0" t="s">
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="3" t="s">
         <v>307</v>
       </c>
@@ -2667,15 +2673,15 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="3" t="s">
-        <v>195</v>
+        <v>321</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="3" t="s">
-        <v>322</v>
+        <v>197</v>
       </c>
       <c r="C140" s="0" t="s">
         <v>323</v>
@@ -2691,69 +2697,77 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="3" t="s">
-        <v>204</v>
+        <v>326</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
-        <v>327</v>
-      </c>
       <c r="B143" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B144" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C143" s="0" t="s">
+      <c r="C144" s="0" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B144" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="C144" s="0" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="3" t="s">
-        <v>92</v>
+        <v>330</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>93</v>
+        <v>331</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C147" s="0" t="s">
-        <v>330</v>
+        <v>94</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>99</v>
+        <v>332</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="3" t="s">
-        <v>331</v>
+        <v>98</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>332</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B150" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C150" s="0" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds button label substitutions for HEATING, COOLING and all 4 event types - adds slot definition to wsport class - updates machine settings to take advantage of translated button label substitutions - adds roaster batch size defaults for machine setups - if different from the system default, use current serial port or current IP host as default on running a machine setup - fixes a case where the MODBUS channel divider got applied to the error value -1 - fixes event button label substitution update on changing event type - persist ET marker size changes correctly - adds translation for SV slider label - Kaleido support: ensure correct order of SC AR and CL AR commands - Kaleido support: sends TP mark event to machine - Kaleido support: hide AT curve, show SV curve - Kaleido support: make palette 1 the default - Kaleido support: fix typo in COOLING button - Kaleido support: sync back main events issued on the machine to Artisan - Kaleido support: adds HS command
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="355">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -169,6 +169,30 @@
     <t xml:space="preserve">Event name (translated if using default event names)</t>
   </si>
   <si>
+    <t xml:space="preserve">\\q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event type 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event type 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event type 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event type 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">\\0</t>
   </si>
   <si>
@@ -239,6 +263,42 @@
   </si>
   <si>
     <t xml:space="preserve">OPEN (translated, respecting button state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTO (translated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUAL (translated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTO (translated, respecting button state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUAL (translated, respecting button state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEATING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COOLING</t>
   </si>
   <si>
     <t xml:space="preserve">COMMANDS</t>
@@ -1158,10 +1218,10 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B45:C45 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A26:A27 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1261,10 +1321,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="1" sqref="B45:C45 B24"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="1" sqref="A26:A27 B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
@@ -1379,13 +1439,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B45:C45 A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26:A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1515,6 +1575,86 @@
       </c>
       <c r="B17" s="0" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1535,11 +1675,11 @@
   </sheetPr>
   <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45:C45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B45" activeCellId="1" sqref="A26:A27 B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1548,32 +1688,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,7 +1721,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>3</v>
@@ -1589,1185 +1729,1185 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="3" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="3" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="3" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="3" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="3" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="3" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="3" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="3" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="3" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="3" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="3" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="3" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="3" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="3" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="3" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="3" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="3" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="3" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="3" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="3" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="3" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="3" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="3" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="3" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="3" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="3" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="3" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="3" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="3" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="3" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="3" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="3" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="3" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="3" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="3" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="3" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="3" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="3" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="3" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="3" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="3" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="3" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="3" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="3" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="3" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="3" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="3" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="3" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="3" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="3" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="3" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="3" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="3" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="3" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="3" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="3" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="3" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="3" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="3" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="3" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="3" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="3" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="3" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="3" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="3" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="3" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="3" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="3" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="3" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="3" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="3" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="3" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="3" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="3" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="3" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="3" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="3" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="3" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="3" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="3" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="3" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="3" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="3" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="3" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="3" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="3" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="3" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="3" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="3" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="3" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="3" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="3" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>327</v>
+        <v>347</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="3" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>329</v>
+        <v>349</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="3" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="3" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="3" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="3" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fixes Santoker Series Fahrenheit mode - fixes missing event name translations (Issue #1181) - fixes issues with the Designer config table (Issue #1173) - fixes TMP1200_0 noise issue (Issue #1175) - fixes Santoker Series machine setup quantifiers to use SV mode - render Ramp/Soak info messages without decimals (Issue #1176) - ensures that rendering of axis respects curve style setting - adds Artisan Command pidSVC(<n>) allowing to specify the SV in C which get's correctly converted to F in Fahrenheit mode - adds IKAWA support
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="357">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -863,6 +863,12 @@
   </si>
   <si>
     <t xml:space="preserve">sets the PID target set value SV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pidSVC(&lt;int&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets the PID target set value SV given in C</t>
   </si>
   <si>
     <t xml:space="preserve">pidRS(&lt;rs&gt;)</t>
@@ -1218,10 +1224,10 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A26:A27 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1321,10 +1327,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="1" sqref="A26:A27 B24"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
@@ -1441,11 +1447,11 @@
   </sheetPr>
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26:A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1673,13 +1679,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B45" activeCellId="1" sqref="A26:A27 B45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C107" activeCellId="0" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -2626,34 +2632,34 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C117" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C117" s="0" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="3" t="s">
-        <v>118</v>
+        <v>300</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>119</v>
+        <v>301</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="3" t="s">
-        <v>300</v>
+        <v>118</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>301</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,17 +2759,17 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
+      <c r="B132" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="C132" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="C132" s="0" t="s">
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="3" t="s">
         <v>329</v>
       </c>
@@ -2821,15 +2827,15 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="3" t="s">
-        <v>217</v>
+        <v>343</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="3" t="s">
-        <v>344</v>
+        <v>217</v>
       </c>
       <c r="C141" s="0" t="s">
         <v>345</v>
@@ -2845,69 +2851,77 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C143" s="0" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="B144" s="3" t="s">
+      <c r="C144" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="B145" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C144" s="0" t="s">
+      <c r="C145" s="0" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B145" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="C145" s="0" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="3" t="s">
-        <v>112</v>
+        <v>352</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>113</v>
+        <v>353</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C148" s="0" t="s">
-        <v>352</v>
+        <v>114</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>119</v>
+        <v>354</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="3" t="s">
-        <v>353</v>
+        <v>118</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>354</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C151" s="0" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allow Multi Event button actions be triggered by Multi Event button actions
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" state="visible" r:id="rId2"/>
@@ -355,7 +355,56 @@
     <t xml:space="preserve">Multiple Event</t>
   </si>
   <si>
-    <t xml:space="preserve">button numbers separated by a comma: 1,2,..</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">button numbers or </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sleep(&lt;float&gt;)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> separated by a comma: 1,2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">sleep(2.5), 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">..</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">triggers other buttons</t>
@@ -1118,7 +1167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1154,6 +1203,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1242,7 +1297,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1344,7 +1399,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.29"/>
@@ -1461,11 +1516,11 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1719,11 +1774,11 @@
   </sheetPr>
   <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C107" activeCellId="0" sqref="C107"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.57"/>
@@ -1790,7 +1845,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>109</v>
       </c>

</xml_diff>

<commit_message>
adds `Artisan Command` `visible(i,b)` to change visibility of button `i` to `b` which has to be an expression which evaluates to a boolean, like 0, 1, false, true, ... (Issue #1301)
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="365">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -970,10 +970,19 @@
     <t xml:space="preserve">resets canvas color</t>
   </si>
   <si>
+    <t xml:space="preserve">sets button i to pressed if value of b is yes, true, t, or 1, otherwise to normal</t>
+  </si>
+  <si>
     <t xml:space="preserve">button(&lt;name&gt;|&lt;bool&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">activates button &lt;name&gt; from { START, CHARGE, DRY, FCs, FCe, SCs, SCe, DROP, COOL, OFF } ; sets calling button to “pressed” if argument is 1 or True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visible(i,b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets button i to visible if value of b is yes, true, t, or 1, otherwise to hidden</t>
   </si>
   <si>
     <t xml:space="preserve">palette(&lt;p&gt;)</t>
@@ -1272,7 +1281,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1374,7 +1383,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.29"/>
@@ -1491,11 +1500,11 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1747,17 +1756,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C151"/>
+  <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C120" activeCellId="0" sqref="C120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="102.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="100.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2711,15 +2720,15 @@
         <v>119</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>120</v>
+        <v>305</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2730,114 +2739,111 @@
         <v>124</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
-        <v>333</v>
-      </c>
       <c r="B133" s="3" t="s">
         <v>334</v>
       </c>
@@ -2846,150 +2852,161 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>336</v>
+      </c>
       <c r="B134" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="3" t="s">
-        <v>222</v>
+        <v>351</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="3" t="s">
-        <v>351</v>
+        <v>222</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C144" s="0" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B145" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="C144" s="0" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="B145" s="3" t="s">
+      <c r="C145" s="0" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B146" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C145" s="0" t="s">
+      <c r="C146" s="0" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B146" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="C146" s="0" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="3" t="s">
-        <v>117</v>
+        <v>360</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>118</v>
+        <v>361</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="C148" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C149" s="0" t="s">
-        <v>359</v>
+        <v>119</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>124</v>
+        <v>362</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="3" t="s">
-        <v>360</v>
+        <v>123</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>361</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C152" s="0" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds machine setup for BeanGo Cube X - updates machine setups for small machines to default to g instead of kg - removes bitmaps from SVG app icon - translation updates
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="367">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t xml:space="preserve">FILL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\R</t>
   </si>
   <si>
     <t xml:space="preserve">RELEASE</t>
@@ -1280,7 +1283,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1382,7 +1385,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.27"/>
@@ -1499,11 +1502,11 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1717,26 +1720,26 @@
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1757,50 +1760,50 @@
   </sheetPr>
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="115.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="115.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="100.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,7 +1811,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>3</v>
@@ -1816,1201 +1819,1201 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- updates BeanCube setup - adds \V (value) and \T (converted temperature value) button label substitutions - adds {TEMP} event value interpreted as temperature in Fahrenheit converted to current temperature mode substitution
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="371">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -319,13 +319,25 @@
     <t xml:space="preserve">COOLING</t>
   </si>
   <si>
+    <t xml:space="preserve">\\V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">event value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">event value interpreted as temperature in Fahrenheit converted to the current temperature mode</t>
+  </si>
+  <si>
     <t xml:space="preserve">COMMANDS</t>
   </si>
   <si>
     <t xml:space="preserve">tn:Note: "{}" can be used as a placeholder, it will be substituted by the current button value plus the offset for \u00B1 event types.  If a placeholder occurs several times in a description/command, all those occurrences are replaced by the value.\n</t>
   </si>
   <si>
-    <t xml:space="preserve">tn:Note: The placeholders {ET}, {BT}, {time}, {ETB}, {BTB}, and {WEIGHTin} will be substituted by the current ET, BT, time, ET background, BT background value and batch size (in g) in Serial/Artisan/CallProgram/MODBUS/S7/WebSocket commands\n</t>
+    <t xml:space="preserve">tn:Note: The placeholders {ET}, {BT}, {time}, {ETB}, {BTB}, {WEIGHTin} and {TEMP} will be substituted by the current ET, BT, time, ET background, BT background value, batch size (in g), event value in F converted to current temperature unit in Serial/Artisan/CallProgram/MODBUS/S7/WebSocket commands\n</t>
   </si>
   <si>
     <t xml:space="preserve">tn:Note: Commands can be sequenced, separated by semicolons like in “&lt;cmd1&gt;;&lt;cmd2&gt;;&lt;cmd3&gt;”\n</t>
@@ -1283,7 +1295,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1385,7 +1397,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.27"/>
@@ -1500,13 +1512,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1740,6 +1752,22 @@
       </c>
       <c r="B30" s="0" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1760,50 +1788,50 @@
   </sheetPr>
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="115.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="124.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="100.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,7 +1839,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>3</v>
@@ -1819,1201 +1847,1201 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="2" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="2" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="2" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="2" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="2" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="2" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="2" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="2" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="2" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="2" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="2" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="2" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="2" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="2" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="2" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="2" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="2" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="2" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="2" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="2" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="2" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="2" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="2" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="2" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="2" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="2" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="2" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="2" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="2" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="2" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="2" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="2" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="2" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="2" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="2" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="2" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="2" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="2" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="2" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="2" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="2" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="2" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="2" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="2" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="2" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="2" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="2" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="2" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="2" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="2" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="2" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="2" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="2" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds support for the to-be-released TMP1202 - allows PID ON command also while not sampling - updates BeanCube X setup
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="373">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -325,10 +325,16 @@
     <t xml:space="preserve">event value</t>
   </si>
   <si>
+    <t xml:space="preserve">\\F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">event value interpreted as temperature in Fahrenheit converted to the current temperature mode</t>
+  </si>
+  <si>
     <t xml:space="preserve">\\T</t>
   </si>
   <si>
-    <t xml:space="preserve">event value interpreted as temperature in Fahrenheit converted to the current temperature mode</t>
+    <t xml:space="preserve">event value interpreted as temperature in Celsius converted to the current temperature mode</t>
   </si>
   <si>
     <t xml:space="preserve">COMMANDS</t>
@@ -337,7 +343,7 @@
     <t xml:space="preserve">tn:Note: "{}" can be used as a placeholder, it will be substituted by the current button value plus the offset for \u00B1 event types.  If a placeholder occurs several times in a description/command, all those occurrences are replaced by the value.\n</t>
   </si>
   <si>
-    <t xml:space="preserve">tn:Note: The placeholders {ET}, {BT}, {time}, {ETB}, {BTB}, {WEIGHTin} and {TEMP} will be substituted by the current ET, BT, time, ET background, BT background value, batch size (in g), event value in F converted to current temperature unit in Serial/Artisan/CallProgram/MODBUS/S7/WebSocket commands\n</t>
+    <t xml:space="preserve">tn:Note: The placeholders {ET}, {BT}, {time}, {ETB}, {BTB}, and {WEIGHTin} will be substituted by the current ET, BT, time, ET background, BT background value, and batch size (in g) in Serial/Artisan/CallProgram/MODBUS/S7/WebSocket commands\n</t>
   </si>
   <si>
     <t xml:space="preserve">tn:Note: Commands can be sequenced, separated by semicolons like in “&lt;cmd1&gt;;&lt;cmd2&gt;;&lt;cmd3&gt;”\n</t>
@@ -1292,10 +1298,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="32:32 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1394,10 +1400,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="32:32 B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.27"/>
@@ -1512,13 +1518,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="32:32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1768,6 +1774,14 @@
       </c>
       <c r="B32" s="0" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1788,50 +1802,50 @@
   </sheetPr>
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="32:32 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="124.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="112.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="100.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,7 +1853,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>3</v>
@@ -1847,1201 +1861,1201 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="2" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="2" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="2" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="2" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="2" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="2" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="2" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="2" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="2" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="2" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="2" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="2" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="2" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="2" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="2" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="2" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="2" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="2" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates translations and K&M UG Control button labels
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="378">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t xml:space="preserve">FILL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISCHARGE</t>
   </si>
   <si>
     <t xml:space="preserve">\\R</t>
@@ -1640,10 +1643,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1860,66 +1863,74 @@
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="1" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
         <v>107</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1953,37 +1964,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,7 +2002,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
@@ -1999,1201 +2010,1201 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="3" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="3" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="3" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="3" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="3" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="3" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="3" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="3" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="3" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- updates some libs - adds translatable labels to some more machine setups
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="379">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t xml:space="preserve">FILL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\D</t>
   </si>
   <si>
     <t xml:space="preserve">DISCHARGE</t>
@@ -1645,8 +1648,8 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1863,74 +1866,74 @@
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1964,37 +1967,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2002,7 +2005,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
@@ -2010,1201 +2013,1201 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="3" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="3" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="3" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="3" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- makes background profile datatable more robust - indicates artisan.plus connection loss more reliable - don't register incomplete roasts in scheduler - makes loading of (broken) profiles more robust - updates matplotlib and other libs - prevents incomplete blends - energy tab improvements  . protocol tool never generates '_:_' entries  . updates protocol duration validator regex to reset Default buttons on clearing entries   . reorganization of signal processing to ensure complete reset to defaults
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" state="visible" r:id="rId3"/>
@@ -745,22 +745,22 @@
     <t xml:space="preserve">PHIDGET PWM Output: turn &lt;channel&gt; on for &lt;millis&gt; milliseconds</t>
   </si>
   <si>
-    <t xml:space="preserve">outhub(&lt;channel&gt;,&lt;value&gt;[,&lt;sn&gt;])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHIDGET HUB PWM Output: &lt;value&gt; in [0-100]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">togglehub(&lt;channel&gt;[,&lt;sn&gt;])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHIDGET HUB PWM Output: toggles &lt;channel&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pulsehub(&lt;channel&gt;,&lt;millis&gt;[,&lt;sn&gt;])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHIDGET HUB PWM Output:  turn &lt;channel&gt; on for &lt;millis&gt; milliseconds</t>
+    <t xml:space="preserve">outhub(&lt;port&gt;,&lt;value&gt;[,&lt;sn&gt;])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHIDGET HUB PWM Output ON port &lt;port&gt; to  &lt;value&gt; in [0-100]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">togglehub(&lt;port&gt;[,&lt;sn&gt;])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHIDGET HUB PWM Output: toggles &lt;port&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pulsehub(&lt;port&gt;,&lt;millis&gt;[,&lt;sn&gt;])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHIDGET HUB PWM Output:  turn &lt;port&gt; ON for &lt;millis&gt; milliseconds</t>
   </si>
   <si>
     <t xml:space="preserve">enabled(c,b[,sn])</t>
@@ -1648,7 +1648,7 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -1954,13 +1954,13 @@
   </sheetPr>
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C66" activeCellId="0" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="112.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="100.36"/>
   </cols>

</xml_diff>

<commit_message>
- raise max event button limits from 4 rows a 30 buttons to 10 rows a 50 buttons - keep custom events ordered by time - fixes regression in Events Editor which broke any edits (after v3.1 got released) - fixes regression introduced in v3.0 which prevented to replay events before CHARGE - adds new flag "Set batch size" to background dialog. If ticked the batch size is taken from the background profile on load while scheduler is off - adds new Artisan Command "setBatchSize(<float>)" to set the batch size. if the given number is negative the batch size is taken from the background profile, if available - adds new Artisan Command "quantifier(n,<bool>)" to toggle quantification per event type
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="383">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -1037,6 +1037,48 @@
   </si>
   <si>
     <t xml:space="preserve">sets playback mode to 0: off, 1: time, 2: BT, 3: ET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantifier(n,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">activate/deactivate quantification per event type </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> from {1,2,3,4}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">setBatchSize(&lt;float&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set the batch size to the given value. If the value is negative, the batch size is taken from the background profile, if any is loaded</t>
   </si>
   <si>
     <t xml:space="preserve">openProperties</t>
@@ -1952,17 +1994,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C153"/>
+  <dimension ref="A1:C155"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C66" activeCellId="0" sqref="C66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C125" activeCellId="0" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="100.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="58.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,25 +3096,25 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="s">
+      <c r="B135" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="B135" s="3" t="s">
+      <c r="C135" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C136" s="1" t="s">
+    </row>
+    <row r="137" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="137" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="3" t="s">
         <v>355</v>
       </c>
@@ -3121,23 +3164,23 @@
     </row>
     <row r="143" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="3" t="s">
-        <v>236</v>
+        <v>367</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="3" t="s">
-        <v>370</v>
+        <v>236</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>371</v>
@@ -3145,69 +3188,85 @@
     </row>
     <row r="146" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="3" t="s">
-        <v>245</v>
+        <v>372</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="B147" s="3" t="s">
-        <v>129</v>
+        <v>374</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>130</v>
+        <v>375</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>374</v>
+        <v>245</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="B149" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="3" t="s">
-        <v>133</v>
+        <v>378</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>134</v>
+        <v>379</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>376</v>
+        <v>132</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="3" t="s">
-        <v>377</v>
+        <v>135</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B154" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- updates IMF control setup - updates pymodbus and PyQt - adds Artisan Commands `ramp` and `playback` - perists the parameters "max. number of custom buttons per row", "button size", "alternative slider layout", "mark last pressed" and "show tooltips" per palette
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="387">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -1039,6 +1039,85 @@
     <t xml:space="preserve">sets playback mode to 0: off, 1: time, 2: BT, 3: ET</t>
   </si>
   <si>
+    <t xml:space="preserve">playback(n,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">toggles playback per event type </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">n </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">from {1,2,3,4}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ramp(n,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">toggles playback ramping per </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">event type </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">n </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">from {1,2,3,4}</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">quantifier(n,&lt;bool&gt;)</t>
   </si>
   <si>
@@ -1241,7 +1320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1277,6 +1356,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1994,10 +2086,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C155"/>
+  <dimension ref="A1:C157"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C125" activeCellId="0" sqref="C125"/>
+      <selection pane="topLeft" activeCell="C124" activeCellId="0" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2005,7 +2097,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="58.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="44.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3112,25 +3204,25 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="s">
+      <c r="B137" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="B137" s="3" t="s">
+      <c r="C137" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="C138" s="1" t="s">
+    </row>
+    <row r="139" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="139" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="3" t="s">
         <v>359</v>
       </c>
@@ -3180,23 +3272,23 @@
     </row>
     <row r="145" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="3" t="s">
-        <v>236</v>
+        <v>371</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="3" t="s">
-        <v>374</v>
+        <v>236</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>375</v>
@@ -3204,69 +3296,85 @@
     </row>
     <row r="148" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>245</v>
+        <v>376</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="1" t="s">
-        <v>377</v>
-      </c>
       <c r="B149" s="3" t="s">
-        <v>129</v>
+        <v>378</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>130</v>
+        <v>379</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="3" t="s">
-        <v>378</v>
+        <v>245</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>381</v>
+      </c>
       <c r="B151" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="3" t="s">
-        <v>133</v>
+        <v>382</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>134</v>
+        <v>383</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>380</v>
+        <v>132</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="3" t="s">
-        <v>381</v>
+        <v>135</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B156" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B157" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- a click in a sliders pane does not move the slider, but only gives it the input focus (a click in a sliders bar still moves the slider to this position) - a click on a sliders lcd give the slider the input focus - a double click on a sliders lcd opens a widget to directly input a new slider value - a right-click on the graph is no longer restricted to a location close to the BT curve and sets the event value from the clicks position in the add event popup on selecting EVENT - events of the foreground profile displayed as Step, Step+ or Combo can be updated by moving them to a new position. Pressing SHIFT restricts the movement in the x or y direction. - numpy update
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="389">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -886,6 +886,32 @@
     <t xml:space="preserve">Artisan Command</t>
   </si>
   <si>
+    <t xml:space="preserve">alarm(n,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">enables/disables alarm number </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">n</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">alarms(&lt;bool&gt;)</t>
   </si>
   <si>
@@ -1086,16 +1112,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">toggles playback ramping per </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">event type </t>
+      <t xml:space="preserve">toggles playback ramping per event type </t>
     </r>
     <r>
       <rPr>
@@ -1104,6 +1121,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">n </t>
     </r>
@@ -1113,6 +1131,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">from {1,2,3,4}</t>
     </r>
@@ -1320,7 +1339,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1356,19 +1375,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2086,10 +2092,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C157"/>
+  <dimension ref="A1:C158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C124" activeCellId="0" sqref="C124"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C98" activeCellId="0" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2901,18 +2907,18 @@
     </row>
     <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="3" t="s">
-        <v>131</v>
+        <v>283</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>132</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="3" t="s">
-        <v>283</v>
+        <v>131</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>284</v>
+        <v>132</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,15 +3059,15 @@
     </row>
     <row r="118" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="3" t="s">
-        <v>133</v>
+        <v>319</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="3" t="s">
-        <v>320</v>
+        <v>133</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>321</v>
@@ -3069,18 +3075,18 @@
     </row>
     <row r="120" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="3" t="s">
-        <v>137</v>
+        <v>322</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>138</v>
+        <v>323</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="3" t="s">
-        <v>322</v>
+        <v>137</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>323</v>
+        <v>138</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3220,17 +3226,17 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="s">
+      <c r="B139" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="B139" s="3" t="s">
+      <c r="C139" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C139" s="1" t="s">
+    </row>
+    <row r="140" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="140" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="3" t="s">
         <v>361</v>
       </c>
@@ -3288,15 +3294,15 @@
     </row>
     <row r="147" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="3" t="s">
-        <v>236</v>
+        <v>375</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>376</v>
+        <v>236</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>377</v>
@@ -3312,69 +3318,77 @@
     </row>
     <row r="150" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C150" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="B151" s="3" t="s">
+      <c r="C151" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B152" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="C152" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B152" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="3" t="s">
-        <v>131</v>
+        <v>384</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>132</v>
+        <v>385</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>384</v>
+        <v>134</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>138</v>
+        <v>386</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="3" t="s">
-        <v>385</v>
+        <v>137</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>386</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B158" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- avoid switching to an empty button using a CMD-<n> shortcut - adds pick and cursor key move for background events - adds pick and move for events rendered in Step+ mode - update all machine settings using MODBUS write for writing to a single register using the more specific writeSingle - updated Artisan Commands pidSV, pidSVC and adjustSV to take floats instead of integers (internal PID) - disable palette switching to empty palettes via number keys to prevent overwriting of current even setup - adds Yoshan YS machine setup - update IMF Control machine setup
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -966,19 +966,19 @@
     <t xml:space="preserve">sets the p-i-d parameters of the PID</t>
   </si>
   <si>
-    <t xml:space="preserve">adjustSV(&lt;int&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">increases or decreases the current target SV value by &lt;int&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pidSV(&lt;int&gt;)</t>
+    <t xml:space="preserve">adjustSV(&lt;float&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">increases or decreases the current target SV value by &lt;float&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pidSV(&lt;float&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">sets the PID target set value SV</t>
   </si>
   <si>
-    <t xml:space="preserve">pidSVC(&lt;int&gt;)</t>
+    <t xml:space="preserve">pidSVC(&lt;float&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">sets the PID target set value SV given in C</t>
@@ -2094,8 +2094,8 @@
   </sheetPr>
   <dimension ref="A1:C158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C98" activeCellId="0" sqref="C98"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C107" activeCellId="0" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
- avoids flicks in ramping event replay by temperature - adds experimental IMF Control 2PID machine setup - enables hi-res internal PID output
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="391">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -731,6 +731,12 @@
   </si>
   <si>
     <t xml:space="preserve">PHIDGET PWM Output: &lt;value&gt; in [0-100]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frequency(&lt;value&gt;[,&lt;sn&gt;])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHIDGET PWM Frequency: &lt;value&gt; in Hz</t>
   </si>
   <si>
     <t xml:space="preserve">toggle(&lt;channel&gt;[,&lt;sn&gt;])</t>
@@ -2092,10 +2098,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:C159"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C107" activeCellId="0" sqref="C107"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C63" activeCellId="0" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2686,17 +2692,17 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
+      <c r="B73" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="C73" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C73" s="1" t="s">
+    </row>
+    <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="3" t="s">
         <v>247</v>
       </c>
@@ -2722,69 +2728,69 @@
     </row>
     <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B78" s="3" t="s">
+    <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="C79" s="1" t="s">
-        <v>130</v>
+        <v>256</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="3" t="s">
-        <v>255</v>
+        <v>137</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>256</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2836,57 +2842,57 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
+      <c r="B91" s="3" t="s">
         <v>269</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>212</v>
+        <v>270</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>272</v>
+        <v>214</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="C94" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="C95" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C96" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2915,18 +2921,18 @@
     </row>
     <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="3" t="s">
-        <v>131</v>
+        <v>285</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>132</v>
+        <v>286</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="3" t="s">
-        <v>285</v>
+        <v>131</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>286</v>
+        <v>132</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3067,15 +3073,15 @@
     </row>
     <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="3" t="s">
-        <v>133</v>
+        <v>321</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="3" t="s">
-        <v>322</v>
+        <v>133</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>323</v>
@@ -3083,18 +3089,18 @@
     </row>
     <row r="121" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="3" t="s">
-        <v>137</v>
+        <v>324</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>138</v>
+        <v>325</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>324</v>
+        <v>137</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>325</v>
+        <v>138</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3234,17 +3240,17 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="s">
+      <c r="B140" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="B140" s="3" t="s">
+      <c r="C140" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="C140" s="1" t="s">
+    </row>
+    <row r="141" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="141" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="3" t="s">
         <v>363</v>
       </c>
@@ -3302,15 +3308,15 @@
     </row>
     <row r="148" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>236</v>
+        <v>377</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="3" t="s">
-        <v>378</v>
+        <v>238</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>379</v>
@@ -3326,69 +3332,77 @@
     </row>
     <row r="151" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="3" t="s">
-        <v>245</v>
+        <v>382</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="1" t="s">
-        <v>383</v>
-      </c>
       <c r="B152" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B153" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C153" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B153" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="3" t="s">
-        <v>131</v>
+        <v>386</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>132</v>
+        <v>387</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>386</v>
+        <v>134</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>138</v>
+        <v>388</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="3" t="s">
-        <v>387</v>
+        <v>137</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>388</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B159" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds configuration to specify the mode (by time, BT or ET) for the playback of the DROP event - adds mixed event playback, by time (for increasing event values) and temperature (for decreasing event values)
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="398">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -1069,6 +1069,12 @@
   </si>
   <si>
     <t xml:space="preserve">sets playback mode to 0: off, 1: time, 2: BT, 3: ET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">playbackdropmode(&lt;int&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets playback DROP mode to 0: off, 1: time, 2: BT, 3: ET</t>
   </si>
   <si>
     <t xml:space="preserve">playback(n,&lt;bool&gt;)</t>
@@ -1587,7 +1593,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="126:126 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1689,7 +1695,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="126:126 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1810,7 +1816,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="1" sqref="126:126 A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2113,10 +2119,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C162"/>
+  <dimension ref="A1:C163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B144" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C152" activeCellId="0" sqref="C152"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A117" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A126" activeCellId="0" sqref="126:126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3263,17 +3269,17 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="s">
+      <c r="B141" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="B141" s="3" t="s">
+      <c r="C141" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="C141" s="1" t="s">
+    </row>
+    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="3" t="s">
         <v>365</v>
       </c>
@@ -3331,15 +3337,15 @@
     </row>
     <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="3" t="s">
-        <v>238</v>
+        <v>379</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="3" t="s">
-        <v>380</v>
+        <v>238</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>381</v>
@@ -3355,26 +3361,26 @@
     </row>
     <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B153" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>377</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="B154" s="3" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>388</v>
@@ -3382,69 +3388,77 @@
     </row>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="3" t="s">
-        <v>367</v>
+        <v>389</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="s">
-        <v>390</v>
-      </c>
       <c r="B156" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B157" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C157" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B157" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="3" t="s">
-        <v>131</v>
+        <v>393</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>132</v>
+        <v>394</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>393</v>
+        <v>134</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>138</v>
+        <v>395</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="3" t="s">
-        <v>394</v>
+        <v>137</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>395</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B163" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fixes machine setups using deprecated MODBUS Command "write" to use the specific "writeSingle" or "writeWord" - reroute the deprecated MODBUS Command "write" to "writeSingle"
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -517,7 +517,7 @@
     <t xml:space="preserve">write(slaveId,register,value) or write([slaveId,register,value],..,[slaveId,register,value])</t>
   </si>
   <si>
-    <t xml:space="preserve">write register: MODBUS function 6 (int) or function 16 (float)</t>
+    <t xml:space="preserve">deprecated: use writeSingle for MODBUS function 6 (int) or writeWord for function 16 (float)</t>
   </si>
   <si>
     <t xml:space="preserve">wcoil(slaveId,register,&lt;bool&gt;)</t>
@@ -1593,7 +1593,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="126:126 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1695,7 +1695,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="126:126 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1816,7 +1816,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="1" sqref="126:126 A28"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2121,15 +2121,15 @@
   </sheetPr>
   <dimension ref="A1:C163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A117" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A126" activeCellId="0" sqref="126:126"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="58.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="69.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="44.82"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
- adds Artisan Command `slider(<int>, <bool>)` to hide/show sliders - further update of SCE Gemma_2IND and Gemma_6-8IND setups
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="400">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -1146,6 +1146,42 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">from {1,2,3,4}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">slider(n,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">show/hide slider per event type </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> from {1,2,3,4}</t>
     </r>
   </si>
   <si>
@@ -2119,17 +2155,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C163"/>
+  <dimension ref="A1:C164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B116" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C129" activeCellId="0" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="69.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="44.82"/>
   </cols>
   <sheetData>
@@ -3277,17 +3313,17 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="s">
+      <c r="B142" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="B142" s="3" t="s">
+      <c r="C142" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C142" s="1" t="s">
+    </row>
+    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="3" t="s">
         <v>367</v>
       </c>
@@ -3345,15 +3381,15 @@
     </row>
     <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="3" t="s">
-        <v>238</v>
+        <v>381</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="3" t="s">
-        <v>382</v>
+        <v>238</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>383</v>
@@ -3369,26 +3405,26 @@
     </row>
     <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B154" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>379</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
+        <v>389</v>
+      </c>
       <c r="B155" s="3" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>390</v>
@@ -3396,69 +3432,77 @@
     </row>
     <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="3" t="s">
-        <v>369</v>
+        <v>391</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="s">
-        <v>392</v>
-      </c>
       <c r="B157" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B158" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C157" s="1" t="s">
+      <c r="C158" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B158" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="3" t="s">
-        <v>131</v>
+        <v>395</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>132</v>
+        <v>396</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>395</v>
+        <v>134</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>138</v>
+        <v>397</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="3" t="s">
-        <v>396</v>
+        <v>137</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>397</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B164" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removes the term "slave" from the project where possible. There remains a small compatibility layer (to be removed in Artisan v3.4) in main.py and modbusport.py to remain compatible for now with older settings and pymodbus lib versions.
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -472,97 +472,180 @@
     <t xml:space="preserve">toggles the state of the button</t>
   </si>
   <si>
-    <t xml:space="preserve">read(slaveID,register)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reads 1 16bit register from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as unsigned integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">readSigned(slaveId,register)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reads 1 16bit register from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as signed integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">readBCD(slaveID,register)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reads 1 16bit register from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as BCD. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">read32(slaveID,register)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reads 2 16bit registers from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as unsigned integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">read32Signed(slaveID,register)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reads 2 16bit registers from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as signed integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">read32BCD(slaveID,register)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reads 2 16bit register from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as BCD. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">readFloat(slaveID,register)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reads 2 16bit registers from slave slaveID using function 3 (Read Multiple Holding Registers) interpreted as float. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">write(slaveId,register,value) or write([slaveId,register,value],..,[slaveId,register,value])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deprecated: use writeSingle for MODBUS function 6 (int) or writeWord for function 16 (float)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wcoil(slaveId,register,&lt;bool&gt;)</t>
+    <t xml:space="preserve">read(deviceID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 1 16bit register from device deviceID using function 3 (Read Multiple Holding Registers) interpreted as unsigned integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">readSigned(deviceID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 1 16bit register from device deviceID using function 3 (Read Multiple Holding Registers) interpreted as signed integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">readBCD(deviceID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 1 16bit register from device deviceID using function 3 (Read Multiple Holding Registers) interpreted as BCD. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read32(deviceID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit registers from device deviceID using function 3 (Read Multiple Holding Registers) interpreted as unsigned integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read32Signed(deviceID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit registers from device deviceID using function 3 (Read Multiple Holding Registers) interpreted as signed integer. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read32BCD(deviceID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit register from device deviceID using function 3 (Read Multiple Holding Registers) interpreted as BCD. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">readFloat(deviceID,register)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads 2 16bit registers from device deviceID using function 3 (Read Multiple Holding Registers) interpreted as float. The result is bound to the placeholder `_` and thus can be accessed in later commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write(deviceID,register,value) or write([deviceID,register,value],..,[deviceID,register,value])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEPRECATED: use writeSingle for MODBUS function 6 (int) or writeWord for function 16 (float)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wcoil(deviceID,register,&lt;bool&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">write coil: MODBUS function 5</t>
   </si>
   <si>
-    <t xml:space="preserve">wcoils(slaveId,register,[&lt;bool&gt;,..,&lt;bool&gt;])</t>
+    <t xml:space="preserve">wcoils(deviceID,register,[&lt;bool&gt;,..,&lt;bool&gt;])</t>
   </si>
   <si>
     <t xml:space="preserve">write coils: MODBUS function 15</t>
   </si>
   <si>
-    <t xml:space="preserve">mwrite(slaveId,register,andMask,orMask) or mwrite(s,r,am,om,v)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mask write register: MODBUS function 22 or simulates function 22 with function 6 and the given value v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">writem(slaveId,register,value) or writem(slaveId,register,[&lt;int&gt;,..,&lt;int&gt;])</t>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">mwrite(deviceID,register,andMask,orMask) or mwrite(</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">deviceID,register,andMask,orMask</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">,value)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">mask write register: MODBUS function 22 or simulates function 22 with function 6 and the given value value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">writem(deviceID,register,value) or writem(deviceID,register,[&lt;int&gt;,..,&lt;int&gt;])</t>
   </si>
   <si>
     <t xml:space="preserve">write registers: MODBUS function 16</t>
   </si>
   <si>
-    <t xml:space="preserve">writeBCD(s,r,v) or writeBCD([s,r,v],..,[s,r,v])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">write 16bit BCD encoded value v to register r of slave s </t>
-  </si>
-  <si>
-    <t xml:space="preserve">writeWord(slaveId,register,value) or writeWord([slaveId,register,value],..,[slaveId,register,value])</t>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">writeBCD(deviceID,register,value) or writeBCD([</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">deviceID,register,value</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">],..,[</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">deviceID,register,value</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">])</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">write 16bit BCD encoded value to register of device with DeviceID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">writeWord(deviceID,register,value) or writeWord([deviceID,register,value],..,[deviceID,register,value])</t>
   </si>
   <si>
     <t xml:space="preserve">write 32bit float to two 16bit int registers: MODBUS function 16</t>
   </si>
   <si>
-    <t xml:space="preserve">writeLong(slaveId,register,value) or writeLong([slaveId,register,value],..,[slaveId,register,value])</t>
+    <t xml:space="preserve">writeLong(deviceID,register,value) or writeLong([deviceID,register,value],..,[deviceID,register,value])</t>
   </si>
   <si>
     <t xml:space="preserve">write 32bit integer to two 16bit int registers: MODBUS function 16</t>
   </si>
   <si>
-    <t xml:space="preserve">writeSingle(slaveId,register,value) or writeSingle([slaveId,register,value],..,[slaveId,register,value])</t>
+    <t xml:space="preserve">writeSingle(deviceID,register,value) or writeSingle([deviceID,register,value],..,[deviceID,register,value])</t>
   </si>
   <si>
     <t xml:space="preserve">write 16bit integer to a single 16bit register: MODBUS function 6 (int)</t>
@@ -1402,7 +1485,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1438,6 +1521,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2157,8 +2247,8 @@
   </sheetPr>
   <dimension ref="A1:C164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B116" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C129" activeCellId="0" sqref="C129"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
adds Artisan Command `replayLookahead`
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="402">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -532,38 +532,7 @@
     <t xml:space="preserve">write coils: MODBUS function 15</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">mwrite(deviceID,register,andMask,orMask) or mwrite(</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">deviceID,register,andMask,orMask</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,value)</t>
-    </r>
+    <t xml:space="preserve">mwrite(deviceID,register,andMask,orMask) or mwrite(deviceID,register,andMask,orMask,value)</t>
   </si>
   <si>
     <t xml:space="preserve">mask write register: MODBUS function 22 or simulates function 22 with function 6 and the given value value</t>
@@ -575,59 +544,7 @@
     <t xml:space="preserve">write registers: MODBUS function 16</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">writeBCD(deviceID,register,value) or writeBCD([</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">deviceID,register,value</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">],..,[</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">deviceID,register,value</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">])</t>
-    </r>
+    <t xml:space="preserve">writeBCD(deviceID,register,value) or writeBCD([deviceID,register,value],..,[deviceID,register,value])</t>
   </si>
   <si>
     <t xml:space="preserve">write 16bit BCD encoded value to register of device with DeviceID </t>
@@ -1088,7 +1005,13 @@
     <t xml:space="preserve">pidLookahead(&lt;int&gt;)</t>
   </si>
   <si>
-    <t xml:space="preserve">sets the PID lookahead</t>
+    <t xml:space="preserve">sets the PID lookahead in seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">replayLookahead(&lt;int&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets the Ramping Event Replay lookahead in seconds</t>
   </si>
   <si>
     <t xml:space="preserve">popup(&lt;msg&gt;[,&lt;int&gt;])</t>
@@ -1485,7 +1408,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1521,13 +1444,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2245,10 +2161,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C164"/>
+  <dimension ref="A1:C165"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B102" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C114" activeCellId="0" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3228,15 +3144,15 @@
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="3" t="s">
-        <v>133</v>
+        <v>323</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="3" t="s">
-        <v>324</v>
+        <v>133</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>325</v>
@@ -3244,18 +3160,18 @@
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>137</v>
+        <v>326</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>138</v>
+        <v>327</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>326</v>
+        <v>137</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>327</v>
+        <v>138</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3411,17 +3327,17 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="s">
+      <c r="B143" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="B143" s="3" t="s">
+      <c r="C143" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="C143" s="1" t="s">
+    </row>
+    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="3" t="s">
         <v>369</v>
       </c>
@@ -3479,15 +3395,15 @@
     </row>
     <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="3" t="s">
-        <v>238</v>
+        <v>383</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="3" t="s">
-        <v>384</v>
+        <v>238</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>385</v>
@@ -3503,26 +3419,26 @@
     </row>
     <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>381</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
+        <v>391</v>
+      </c>
       <c r="B156" s="3" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>392</v>
@@ -3530,69 +3446,77 @@
     </row>
     <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="3" t="s">
-        <v>371</v>
+        <v>393</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="s">
-        <v>394</v>
-      </c>
       <c r="B158" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B159" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="C159" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B159" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="3" t="s">
-        <v>131</v>
+        <v>397</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>132</v>
+        <v>398</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>397</v>
+        <v>134</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>138</v>
+        <v>399</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="3" t="s">
-        <v>398</v>
+        <v>137</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>399</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B165" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds `shellyrelay` IO Command to switch Shelly Plugs on/off - updated libs - updated translations
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="404">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -686,6 +686,12 @@
   </si>
   <si>
     <t xml:space="preserve">sends &lt;value&gt; to &lt;target&gt; via the Kaleido Serial or Network protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shellyrelay(n,b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switches Shelly plug number &lt;n&gt; ON if b is true or 1, and OFF otherwise</t>
   </si>
   <si>
     <t xml:space="preserve">Hottop Heater</t>
@@ -2161,10 +2167,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C165"/>
+  <dimension ref="A1:C166"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B102" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C114" activeCellId="0" sqref="C114"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2626,7 +2632,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+      <c r="B58" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -2645,29 +2651,29 @@
       <c r="A60" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="C60" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C61" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="C62" s="1" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2678,11 +2684,11 @@
       <c r="B63" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="C63" s="1" t="s">
+    </row>
+    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="3" t="s">
         <v>226</v>
       </c>
@@ -2763,17 +2769,17 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
+      <c r="B74" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="C74" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C74" s="1" t="s">
+    </row>
+    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="3" t="s">
         <v>249</v>
       </c>
@@ -2799,69 +2805,69 @@
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B79" s="3" t="s">
+    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="C80" s="1" t="s">
-        <v>130</v>
+        <v>258</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="3" t="s">
-        <v>257</v>
+        <v>137</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>258</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2913,16 +2919,16 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="s">
+      <c r="B92" s="3" t="s">
         <v>271</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>212</v>
+        <v>272</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>214</v>
@@ -2930,40 +2936,40 @@
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>274</v>
+        <v>216</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="C95" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="C96" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2992,18 +2998,18 @@
     </row>
     <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="3" t="s">
-        <v>131</v>
+        <v>287</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>132</v>
+        <v>288</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="3" t="s">
-        <v>287</v>
+        <v>131</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>288</v>
+        <v>132</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3152,15 +3158,15 @@
     </row>
     <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="3" t="s">
-        <v>133</v>
+        <v>325</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>326</v>
+        <v>133</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>327</v>
@@ -3168,18 +3174,18 @@
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>137</v>
+        <v>328</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>138</v>
+        <v>329</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="3" t="s">
-        <v>328</v>
+        <v>137</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>329</v>
+        <v>138</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3335,17 +3341,17 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="s">
+      <c r="B144" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="C144" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="C144" s="1" t="s">
+    </row>
+    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="3" t="s">
         <v>371</v>
       </c>
@@ -3403,15 +3409,15 @@
     </row>
     <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="3" t="s">
-        <v>238</v>
+        <v>385</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="3" t="s">
-        <v>386</v>
+        <v>240</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>387</v>
@@ -3427,26 +3433,26 @@
     </row>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="3" t="s">
-        <v>247</v>
+        <v>390</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="s">
-        <v>391</v>
-      </c>
       <c r="B156" s="3" t="s">
-        <v>383</v>
+        <v>249</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
+        <v>393</v>
+      </c>
       <c r="B157" s="3" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>394</v>
@@ -3454,69 +3460,77 @@
     </row>
     <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="3" t="s">
-        <v>373</v>
+        <v>395</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="s">
-        <v>396</v>
-      </c>
       <c r="B159" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B160" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="C160" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B160" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="3" t="s">
-        <v>131</v>
+        <v>399</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>132</v>
+        <v>400</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>399</v>
+        <v>134</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>138</v>
+        <v>401</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="3" t="s">
-        <v>400</v>
+        <v>137</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>401</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B166" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- 2DOF PID implementation adding parameters beta and gamma allowing for PoM and DoM in addition to PoE and DoE; defaults to the classic PoE/DoE incl. integral limit adjustment to beta - adds Artisan Command `pidWeights` to set beta and gamma - adds bump-less transfer between MANUAL (PID OFF) and AUTO (PID ON) mode, by setting SV to PV while OFF - makes derivative filter (IIR SOS) respecting the sampling interval - adds output filter (IIR SOS) respecting the sampling interval - adds SV FIR filter only active in background follow mode
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="406">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -976,6 +976,12 @@
   </si>
   <si>
     <t xml:space="preserve">sets the p-i-d parameters of the PID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pidWeights(&lt;beta&gt;,&lt;gamma&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets the beta and gamma parameters of the PID</t>
   </si>
   <si>
     <t xml:space="preserve">adjustSV(&lt;float&gt;)</t>
@@ -2167,10 +2173,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C166"/>
+  <dimension ref="A1:C167"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C109" activeCellId="0" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3166,15 +3172,15 @@
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>133</v>
+        <v>327</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>328</v>
+        <v>133</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>329</v>
@@ -3182,18 +3188,18 @@
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="3" t="s">
-        <v>137</v>
+        <v>330</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>138</v>
+        <v>331</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="3" t="s">
-        <v>330</v>
+        <v>137</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>331</v>
+        <v>138</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3349,17 +3355,17 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="s">
+      <c r="B145" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="B145" s="3" t="s">
+      <c r="C145" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="C145" s="1" t="s">
+    </row>
+    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="3" t="s">
         <v>373</v>
       </c>
@@ -3417,15 +3423,15 @@
     </row>
     <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="3" t="s">
-        <v>240</v>
+        <v>387</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="3" t="s">
-        <v>388</v>
+        <v>240</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>389</v>
@@ -3441,26 +3447,26 @@
     </row>
     <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B157" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>385</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
+        <v>395</v>
+      </c>
       <c r="B158" s="3" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>396</v>
@@ -3468,69 +3474,77 @@
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="3" t="s">
-        <v>375</v>
+        <v>397</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="s">
-        <v>398</v>
-      </c>
       <c r="B160" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B161" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C160" s="1" t="s">
+      <c r="C161" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B161" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="3" t="s">
-        <v>131</v>
+        <v>401</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>132</v>
+        <v>402</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>401</v>
+        <v>134</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>138</v>
+        <v>403</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="3" t="s">
-        <v>402</v>
+        <v>137</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>403</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B167" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enable keyboard shortcut J  to toggle replay in production mode
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -1086,7 +1086,7 @@
     <t xml:space="preserve">playbackmode(&lt;int&gt;)</t>
   </si>
   <si>
-    <t xml:space="preserve">sets playback mode to 0: off, 1: time, 2: BT, 3: ET</t>
+    <t xml:space="preserve">sets playback mode to 0: off, 1: time, 2: BT, 3: ET; 4: BT/time; 5: ET/time</t>
   </si>
   <si>
     <t xml:space="preserve">playbackdropmode(&lt;int&gt;)</t>
@@ -2175,8 +2175,8 @@
   </sheetPr>
   <dimension ref="A1:C167"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B105" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C131" activeCellId="0" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
- updates CN translations - adds slider(5,<bool>) Artisan Command to toggle visibility of the SV Slider - extended MPL default font mappings for the languages AR, HE, KR, zh_CN, zh_TW on Linux
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -13,6 +13,9 @@
     <sheet name="Labels" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Commands" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">Commands!$C$132</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1199,7 +1202,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> from {1,2,3,4}</t>
+      <t xml:space="preserve"> from {1,2,3,4}; n=5 toggles the PID SV slider visibility</t>
     </r>
   </si>
   <si>
@@ -2175,8 +2178,8 @@
   </sheetPr>
   <dimension ref="A1:C167"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B105" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C131" activeCellId="0" sqref="C131"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B113" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C132" activeCellId="0" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
- German translation update - fixes canvas color handling - adds alarm documentation to alarm trigger message - adds Artisan Command pidSVbuttons(<bool>) (Issue #2121) - fixes lrelease path for latest setuptools
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Commands" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">Commands!$C$132</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">Commands!$C$133</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="408">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -1003,6 +1003,12 @@
   </si>
   <si>
     <t xml:space="preserve">sets the PID target set value SV given in C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pidSVbuttons(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggles the visibility of the PID SV buttons</t>
   </si>
   <si>
     <t xml:space="preserve">pidRS(&lt;rs&gt;)</t>
@@ -2176,10 +2182,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C167"/>
+  <dimension ref="A1:C168"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B113" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C132" activeCellId="0" sqref="C132"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B104" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C113" activeCellId="0" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3183,15 +3189,15 @@
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>133</v>
+        <v>329</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="3" t="s">
-        <v>330</v>
+        <v>133</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>331</v>
@@ -3199,18 +3205,18 @@
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="3" t="s">
-        <v>137</v>
+        <v>332</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>138</v>
+        <v>333</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="3" t="s">
-        <v>332</v>
+        <v>137</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>333</v>
+        <v>138</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3366,17 +3372,17 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="s">
+      <c r="B146" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="B146" s="3" t="s">
+      <c r="C146" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="C146" s="1" t="s">
+    </row>
+    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="3" t="s">
         <v>375</v>
       </c>
@@ -3434,15 +3440,15 @@
     </row>
     <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="3" t="s">
-        <v>240</v>
+        <v>389</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="3" t="s">
-        <v>390</v>
+        <v>240</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>391</v>
@@ -3458,26 +3464,26 @@
     </row>
     <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B158" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>387</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="B159" s="3" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>398</v>
@@ -3485,69 +3491,77 @@
     </row>
     <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="3" t="s">
-        <v>377</v>
+        <v>399</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="s">
-        <v>400</v>
-      </c>
       <c r="B161" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B162" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="C162" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B162" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="3" t="s">
-        <v>131</v>
+        <v>403</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>132</v>
+        <v>404</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>403</v>
+        <v>134</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>138</v>
+        <v>405</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="3" t="s">
-        <v>404</v>
+        <v>137</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>405</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B168" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>